<commit_message>
updated the excel sheed December8
</commit_message>
<xml_diff>
--- a/Companies_Apply_Status_Sheet.xlsx
+++ b/Companies_Apply_Status_Sheet.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BF8E005-FF79-4A18-8A09-0003B0D06757}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="10725"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="10725" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="704" uniqueCount="521">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="706" uniqueCount="520">
   <si>
     <t>SLNo</t>
   </si>
@@ -1414,9 +1415,6 @@
     <t>https://www.linkedin.com/jobs/search/?alertAction=viewjobs&amp;currentJobId=986139116&amp;f_E=2&amp;keywords=technical%20project%20manager&amp;location=United%20States&amp;locationId=us%3A0&amp;start=25</t>
   </si>
   <si>
-    <t>unable to upload resume</t>
-  </si>
-  <si>
     <t>https://careers.google.com/jobs/results/6525107425837056-technical-program-manager-university-graduate/?src=Online%2FLinkedIn%2Flinkedin_us&amp;utm_campaign=contract&amp;utm_medium=jobposting&amp;utm_source=linkedin</t>
   </si>
   <si>
@@ -1492,9 +1490,6 @@
     <t>https://blackknight.wd1.myworkdayjobs.com/BKC/login?redirect=%2FBKC%2Fjob%2FJacksonville-FL%2FProject-Manager-I---Technical_2018-543-2%2Fapply%3Fsource%3Dlinkedin</t>
   </si>
   <si>
-    <t>link opens a blank page</t>
-  </si>
-  <si>
     <t>https://www.linkedin.com/jobs/view/993929684/?recommendedFlavor=HIDDEN_GEM&amp;trk=d_flagship3_job_home_savedjobs</t>
   </si>
   <si>
@@ -1525,17 +1520,10 @@
     <t>https://www.linkedin.com/jobs/view/792630393/?recommendedFlavor=SCHOOL_RECRUIT&amp;trk=d_flagship3_job_home_savedjobs</t>
   </si>
   <si>
-    <t>ID: 7104BR
-other questions****</t>
-  </si>
-  <si>
     <t>https://sjobs.brassring.com/TGnewUI/Search/home/HomeWithPreLoad?PageType=JobDetails&amp;partnerid=25811&amp;siteid=5185&amp;areq=7104BR#jobDetails=410516_5185</t>
   </si>
   <si>
     <t>Amazon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Job ID 679696  </t>
   </si>
   <si>
     <t>SantaBarbara, CA</t>
@@ -1630,16 +1618,29 @@
   </si>
   <si>
     <t>blank page</t>
+  </si>
+  <si>
+    <t>unable to upload resume
+SB: Submitted might be due to access issues</t>
+  </si>
+  <si>
+    <t>link opens a blank page
+SB: Submitted the application</t>
+  </si>
+  <si>
+    <t>ID: 7104BR
+other questions****
+SB: used the exsiting account and completed thee process</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1802,7 +1803,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1861,6 +1862,8 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2134,23 +2137,23 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
       <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
       <selection activeCell="A7" sqref="A7"/>
-      <selection pane="topRight" activeCell="D81" sqref="D81"/>
+      <selection pane="topRight" activeCell="J72" sqref="J72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.7109375" customWidth="1"/>
@@ -2168,7 +2171,7 @@
     <col min="15" max="15" width="30.42578125" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2215,7 +2218,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -2248,7 +2251,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="4">
         <v>43385</v>
@@ -2275,7 +2278,7 @@
       <c r="N3" s="2"/>
       <c r="O3" s="6"/>
     </row>
-    <row r="4" spans="1:15" ht="45">
+    <row r="4" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="6" t="s">
@@ -2302,7 +2305,7 @@
       <c r="N4" s="2"/>
       <c r="O4" s="6"/>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="6" t="s">
@@ -2325,7 +2328,7 @@
       <c r="N5" s="2"/>
       <c r="O5" s="6"/>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="6" t="s">
@@ -2348,7 +2351,7 @@
       <c r="N6" s="2"/>
       <c r="O6" s="6"/>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="6" t="s">
@@ -2367,7 +2370,7 @@
       <c r="N7" s="2"/>
       <c r="O7" s="6"/>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="6" t="s">
@@ -2390,7 +2393,7 @@
       <c r="N8" s="2"/>
       <c r="O8" s="6"/>
     </row>
-    <row r="9" spans="1:15" ht="45">
+    <row r="9" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="6" t="s">
@@ -2415,7 +2418,7 @@
       <c r="N9" s="2"/>
       <c r="O9" s="6"/>
     </row>
-    <row r="10" spans="1:15" ht="45">
+    <row r="10" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="6" t="s">
@@ -2440,7 +2443,7 @@
       <c r="N10" s="2"/>
       <c r="O10" s="6"/>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="6" t="s">
@@ -2463,7 +2466,7 @@
       <c r="N11" s="2"/>
       <c r="O11" s="6"/>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="6" t="s">
@@ -2486,7 +2489,7 @@
       <c r="N12" s="2"/>
       <c r="O12" s="6"/>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="6" t="s">
@@ -2509,7 +2512,7 @@
       <c r="N13" s="2"/>
       <c r="O13" s="6"/>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="4">
         <v>43430</v>
@@ -2536,7 +2539,7 @@
       </c>
       <c r="O14" s="6"/>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="4">
         <v>43430</v>
@@ -2561,7 +2564,7 @@
       <c r="N15" s="2"/>
       <c r="O15" s="6"/>
     </row>
-    <row r="16" spans="1:15">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="4">
         <v>43430</v>
@@ -2586,7 +2589,7 @@
       <c r="N16" s="2"/>
       <c r="O16" s="6"/>
     </row>
-    <row r="17" spans="1:15">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="4">
         <v>43430</v>
@@ -2611,7 +2614,7 @@
       <c r="N17" s="2"/>
       <c r="O17" s="6"/>
     </row>
-    <row r="18" spans="1:15">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="4">
         <v>43430</v>
@@ -2636,7 +2639,7 @@
       <c r="N18" s="2"/>
       <c r="O18" s="6"/>
     </row>
-    <row r="19" spans="1:15" ht="60">
+    <row r="19" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="4">
         <v>43430</v>
@@ -2663,7 +2666,7 @@
       <c r="N19" s="2"/>
       <c r="O19" s="6"/>
     </row>
-    <row r="20" spans="1:15" ht="30">
+    <row r="20" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="4">
         <v>43430</v>
@@ -2694,7 +2697,7 @@
       </c>
       <c r="O20" s="6"/>
     </row>
-    <row r="21" spans="1:15" ht="45">
+    <row r="21" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="4">
         <v>43430</v>
@@ -2725,7 +2728,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="22" spans="1:15">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="4">
         <v>43430</v>
@@ -2750,7 +2753,7 @@
       <c r="N22" s="2"/>
       <c r="O22" s="6"/>
     </row>
-    <row r="23" spans="1:15" ht="60">
+    <row r="23" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="4">
         <v>43430</v>
@@ -2785,7 +2788,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="49.5" customHeight="1">
+    <row r="24" spans="1:15" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="4">
         <v>43431</v>
@@ -2820,7 +2823,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="25" spans="1:15" ht="49.5" customHeight="1">
+    <row r="25" spans="1:15" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="4">
         <v>43430</v>
@@ -2855,7 +2858,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="26" spans="1:15" ht="75">
+    <row r="26" spans="1:15" ht="75" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="4">
         <v>43430</v>
@@ -2888,7 +2891,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="27" spans="1:15" s="25" customFormat="1" ht="75">
+    <row r="27" spans="1:15" s="25" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A27" s="22"/>
       <c r="B27" s="23">
         <v>43430</v>
@@ -2921,7 +2924,7 @@
       <c r="N27" s="22"/>
       <c r="O27" s="24"/>
     </row>
-    <row r="28" spans="1:15" ht="120">
+    <row r="28" spans="1:15" ht="120" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="4">
         <v>43430</v>
@@ -2954,7 +2957,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="29" spans="1:15" ht="90">
+    <row r="29" spans="1:15" ht="90" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="4">
         <v>43431</v>
@@ -2983,7 +2986,7 @@
       <c r="N29" s="2"/>
       <c r="O29" s="6"/>
     </row>
-    <row r="30" spans="1:15" ht="45">
+    <row r="30" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="4">
         <v>43431</v>
@@ -3012,7 +3015,7 @@
       <c r="N30" s="3"/>
       <c r="O30" s="6"/>
     </row>
-    <row r="31" spans="1:15" ht="105">
+    <row r="31" spans="1:15" ht="105" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="4">
         <v>43431</v>
@@ -3045,7 +3048,7 @@
       </c>
       <c r="O31" s="6"/>
     </row>
-    <row r="32" spans="1:15" ht="30">
+    <row r="32" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="4">
         <v>43431</v>
@@ -3080,7 +3083,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="33" spans="1:15" ht="45">
+    <row r="33" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" s="4">
         <v>43431</v>
@@ -3107,7 +3110,7 @@
       <c r="N33" s="3"/>
       <c r="O33" s="6"/>
     </row>
-    <row r="34" spans="1:15" ht="75">
+    <row r="34" spans="1:15" ht="75" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="4">
         <v>43431</v>
@@ -3136,7 +3139,7 @@
       <c r="N34" s="3"/>
       <c r="O34" s="6"/>
     </row>
-    <row r="35" spans="1:15" ht="75">
+    <row r="35" spans="1:15" ht="75" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="B35" s="4">
         <v>43431</v>
@@ -3167,7 +3170,7 @@
       <c r="N35" s="3"/>
       <c r="O35" s="6"/>
     </row>
-    <row r="36" spans="1:15" ht="255">
+    <row r="36" spans="1:15" ht="255" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
       <c r="B36" s="4">
         <v>43431</v>
@@ -3204,7 +3207,7 @@
       </c>
       <c r="O36" s="6"/>
     </row>
-    <row r="37" spans="1:15" ht="60">
+    <row r="37" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
       <c r="B37" s="4">
         <v>43432</v>
@@ -3235,7 +3238,7 @@
       <c r="N37" s="3"/>
       <c r="O37" s="6"/>
     </row>
-    <row r="38" spans="1:15" ht="60">
+    <row r="38" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" s="4">
         <v>43432</v>
@@ -3264,7 +3267,7 @@
       <c r="N38" s="3"/>
       <c r="O38" s="6"/>
     </row>
-    <row r="39" spans="1:15" ht="60">
+    <row r="39" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="4">
         <v>43432</v>
@@ -3293,7 +3296,7 @@
       <c r="N39" s="3"/>
       <c r="O39" s="6"/>
     </row>
-    <row r="40" spans="1:15" ht="60">
+    <row r="40" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
       <c r="B40" s="4">
         <v>43432</v>
@@ -3322,7 +3325,7 @@
       <c r="N40" s="3"/>
       <c r="O40" s="6"/>
     </row>
-    <row r="41" spans="1:15" ht="135">
+    <row r="41" spans="1:15" ht="135" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
       <c r="B41" s="4">
         <v>43432</v>
@@ -3357,7 +3360,7 @@
       </c>
       <c r="O41" s="6"/>
     </row>
-    <row r="42" spans="1:15" ht="60">
+    <row r="42" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
       <c r="B42" s="4">
         <v>43432</v>
@@ -3388,7 +3391,7 @@
       <c r="N42" s="3"/>
       <c r="O42" s="6"/>
     </row>
-    <row r="43" spans="1:15" ht="60.75">
+    <row r="43" spans="1:15" ht="60.75" x14ac:dyDescent="0.3">
       <c r="A43" s="2"/>
       <c r="B43" s="4">
         <v>43432</v>
@@ -3421,7 +3424,7 @@
       <c r="N43" s="3"/>
       <c r="O43" s="6"/>
     </row>
-    <row r="44" spans="1:15" ht="60">
+    <row r="44" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
       <c r="B44" s="4">
         <v>43432</v>
@@ -3450,7 +3453,7 @@
       <c r="N44" s="3"/>
       <c r="O44" s="6"/>
     </row>
-    <row r="45" spans="1:15" ht="75">
+    <row r="45" spans="1:15" ht="75" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
       <c r="B45" s="4">
         <v>43432</v>
@@ -3479,7 +3482,7 @@
       <c r="N45" s="3"/>
       <c r="O45" s="6"/>
     </row>
-    <row r="46" spans="1:15" ht="45">
+    <row r="46" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
       <c r="B46" s="4">
         <v>43432</v>
@@ -3516,7 +3519,7 @@
       </c>
       <c r="O46" s="6"/>
     </row>
-    <row r="47" spans="1:15" ht="51" customHeight="1">
+    <row r="47" spans="1:15" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
       <c r="B47" s="4">
         <v>43433</v>
@@ -3553,7 +3556,7 @@
       </c>
       <c r="O47" s="6"/>
     </row>
-    <row r="48" spans="1:15" ht="30">
+    <row r="48" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
       <c r="B48" s="4">
         <v>43433</v>
@@ -3584,7 +3587,7 @@
       <c r="N48" s="3"/>
       <c r="O48" s="6"/>
     </row>
-    <row r="49" spans="1:15" ht="30">
+    <row r="49" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
       <c r="B49" s="4">
         <v>43433</v>
@@ -3615,7 +3618,7 @@
       <c r="N49" s="3"/>
       <c r="O49" s="6"/>
     </row>
-    <row r="50" spans="1:15" ht="30">
+    <row r="50" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="2"/>
       <c r="B50" s="4">
         <v>43433</v>
@@ -3646,7 +3649,7 @@
       <c r="N50" s="3"/>
       <c r="O50" s="6"/>
     </row>
-    <row r="51" spans="1:15" ht="30">
+    <row r="51" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="2"/>
       <c r="B51" s="4">
         <v>43433</v>
@@ -3675,7 +3678,7 @@
       <c r="N51" s="3"/>
       <c r="O51" s="6"/>
     </row>
-    <row r="52" spans="1:15" ht="30">
+    <row r="52" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="2"/>
       <c r="B52" s="4">
         <v>43433</v>
@@ -3704,7 +3707,7 @@
       <c r="N52" s="3"/>
       <c r="O52" s="6"/>
     </row>
-    <row r="53" spans="1:15" ht="45">
+    <row r="53" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A53" s="2"/>
       <c r="B53" s="4">
         <v>43433</v>
@@ -3733,7 +3736,7 @@
       <c r="N53" s="3"/>
       <c r="O53" s="6"/>
     </row>
-    <row r="54" spans="1:15" ht="90">
+    <row r="54" spans="1:15" ht="90" x14ac:dyDescent="0.25">
       <c r="A54" s="2"/>
       <c r="B54" s="4">
         <v>43433</v>
@@ -3766,7 +3769,7 @@
       </c>
       <c r="O54" s="6"/>
     </row>
-    <row r="55" spans="1:15" ht="90">
+    <row r="55" spans="1:15" ht="90" x14ac:dyDescent="0.25">
       <c r="A55" s="2"/>
       <c r="B55" s="4">
         <v>43434</v>
@@ -3801,7 +3804,7 @@
       </c>
       <c r="O55" s="6"/>
     </row>
-    <row r="56" spans="1:15" ht="60">
+    <row r="56" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A56" s="2"/>
       <c r="B56" s="4">
         <v>43434</v>
@@ -3830,7 +3833,7 @@
       <c r="N56" s="3"/>
       <c r="O56" s="6"/>
     </row>
-    <row r="57" spans="1:15" ht="42.75" customHeight="1">
+    <row r="57" spans="1:15" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="2"/>
       <c r="B57" s="4">
         <v>43434</v>
@@ -3865,7 +3868,7 @@
       </c>
       <c r="O57" s="6"/>
     </row>
-    <row r="58" spans="1:15" ht="60">
+    <row r="58" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A58" s="2"/>
       <c r="B58" s="4">
         <v>43434</v>
@@ -3894,7 +3897,7 @@
       <c r="N58" s="3"/>
       <c r="O58" s="6"/>
     </row>
-    <row r="59" spans="1:15" ht="42" customHeight="1">
+    <row r="59" spans="1:15" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="2"/>
       <c r="B59" s="4">
         <v>43434</v>
@@ -3923,7 +3926,7 @@
       <c r="N59" s="3"/>
       <c r="O59" s="6"/>
     </row>
-    <row r="60" spans="1:15" ht="60">
+    <row r="60" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A60" s="2"/>
       <c r="B60" s="4">
         <v>43434</v>
@@ -3952,7 +3955,7 @@
       <c r="N60" s="3"/>
       <c r="O60" s="6"/>
     </row>
-    <row r="61" spans="1:15" ht="60">
+    <row r="61" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A61" s="2"/>
       <c r="B61" s="4">
         <v>43434</v>
@@ -3983,32 +3986,32 @@
       <c r="N61" s="3"/>
       <c r="O61" s="6"/>
     </row>
-    <row r="62" spans="1:15" ht="43.5" customHeight="1">
+    <row r="62" spans="1:15" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="2"/>
-      <c r="B62" s="4">
+      <c r="B62" s="28">
         <v>43434</v>
       </c>
-      <c r="C62" s="19" t="s">
+      <c r="C62" s="26" t="s">
         <v>408</v>
       </c>
-      <c r="D62" s="18" t="s">
+      <c r="D62" s="29" t="s">
         <v>446</v>
       </c>
-      <c r="E62" s="19" t="s">
+      <c r="E62" s="26" t="s">
         <v>447</v>
       </c>
-      <c r="F62" s="18"/>
-      <c r="G62" s="18"/>
-      <c r="H62" s="18"/>
-      <c r="I62" s="18"/>
-      <c r="J62" s="18" t="s">
-        <v>449</v>
+      <c r="F62" s="29"/>
+      <c r="G62" s="29"/>
+      <c r="H62" s="29"/>
+      <c r="I62" s="29"/>
+      <c r="J62" s="26" t="s">
+        <v>517</v>
       </c>
       <c r="K62" s="6" t="s">
         <v>448</v>
       </c>
       <c r="L62" s="8" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="M62" s="3" t="s">
         <v>13</v>
@@ -4018,19 +4021,19 @@
       </c>
       <c r="O62" s="6"/>
     </row>
-    <row r="63" spans="1:15" ht="75">
+    <row r="63" spans="1:15" ht="75" x14ac:dyDescent="0.25">
       <c r="A63" s="2"/>
       <c r="B63" s="4">
         <v>43434</v>
       </c>
       <c r="C63" s="6" t="s">
+        <v>450</v>
+      </c>
+      <c r="D63" s="2" t="s">
         <v>451</v>
       </c>
-      <c r="D63" s="2" t="s">
+      <c r="E63" s="6" t="s">
         <v>452</v>
-      </c>
-      <c r="E63" s="6" t="s">
-        <v>453</v>
       </c>
       <c r="F63" s="2"/>
       <c r="G63" s="2"/>
@@ -4038,28 +4041,28 @@
       <c r="I63" s="2"/>
       <c r="J63" s="2"/>
       <c r="K63" s="6" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="L63" s="6" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="M63" s="2"/>
       <c r="N63" s="3"/>
       <c r="O63" s="6"/>
     </row>
-    <row r="64" spans="1:15" ht="51" customHeight="1">
+    <row r="64" spans="1:15" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="2"/>
       <c r="B64" s="4">
         <v>43434</v>
       </c>
       <c r="C64" s="19" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="D64" s="18" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="E64" s="19" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="F64" s="18"/>
       <c r="G64" s="18"/>
@@ -4067,26 +4070,26 @@
       <c r="I64" s="18"/>
       <c r="J64" s="18"/>
       <c r="K64" s="19" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="L64" s="6"/>
       <c r="M64" s="2"/>
       <c r="N64" s="3"/>
       <c r="O64" s="6"/>
     </row>
-    <row r="65" spans="1:15" ht="51" customHeight="1">
+    <row r="65" spans="1:15" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="2"/>
       <c r="B65" s="4">
         <v>43434</v>
       </c>
       <c r="C65" s="6" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="E65" s="6" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="F65" s="2" t="s">
         <v>27</v>
@@ -4096,28 +4099,28 @@
       <c r="I65" s="2"/>
       <c r="J65" s="2"/>
       <c r="K65" s="6" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="L65" s="6" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="M65" s="2"/>
       <c r="N65" s="3"/>
       <c r="O65" s="6"/>
     </row>
-    <row r="66" spans="1:15" ht="30">
+    <row r="66" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A66" s="2"/>
       <c r="B66" s="4">
         <v>43434</v>
       </c>
       <c r="C66" s="6" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="D66" s="2" t="s">
         <v>33</v>
       </c>
       <c r="E66" s="6" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="F66" s="2" t="s">
         <v>31</v>
@@ -4127,39 +4130,39 @@
       <c r="I66" s="2"/>
       <c r="J66" s="2"/>
       <c r="K66" s="6" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="L66" s="6"/>
       <c r="M66" s="2"/>
       <c r="N66" s="3"/>
       <c r="O66" s="6"/>
     </row>
-    <row r="67" spans="1:15" ht="40.5" customHeight="1">
+    <row r="67" spans="1:15" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="2"/>
       <c r="B67" s="4">
         <v>43434</v>
       </c>
       <c r="C67" s="6" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="E67" s="6" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="F67" s="2"/>
       <c r="G67" s="2"/>
       <c r="H67" s="2"/>
       <c r="I67" s="2"/>
       <c r="J67" s="2" t="s">
+        <v>467</v>
+      </c>
+      <c r="K67" s="6" t="s">
+        <v>465</v>
+      </c>
+      <c r="L67" s="6" t="s">
         <v>468</v>
-      </c>
-      <c r="K67" s="6" t="s">
-        <v>466</v>
-      </c>
-      <c r="L67" s="6" t="s">
-        <v>469</v>
       </c>
       <c r="M67" s="3" t="s">
         <v>13</v>
@@ -4169,40 +4172,44 @@
       </c>
       <c r="O67" s="6"/>
     </row>
-    <row r="68" spans="1:15" ht="45">
+    <row r="68" spans="1:15" ht="75" x14ac:dyDescent="0.25">
       <c r="A68" s="2"/>
-      <c r="B68" s="4">
+      <c r="B68" s="28">
         <v>43441</v>
       </c>
-      <c r="C68" s="19" t="s">
+      <c r="C68" s="26" t="s">
+        <v>469</v>
+      </c>
+      <c r="D68" s="29" t="s">
         <v>470</v>
       </c>
-      <c r="D68" s="18" t="s">
+      <c r="E68" s="26" t="s">
         <v>471</v>
       </c>
-      <c r="E68" s="19" t="s">
+      <c r="F68" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="G68" s="29"/>
+      <c r="H68" s="29"/>
+      <c r="I68" s="29"/>
+      <c r="J68" s="26" t="s">
+        <v>518</v>
+      </c>
+      <c r="K68" s="6" t="s">
         <v>472</v>
       </c>
-      <c r="F68" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="G68" s="18"/>
-      <c r="H68" s="18"/>
-      <c r="I68" s="18"/>
-      <c r="J68" s="18" t="s">
-        <v>475</v>
-      </c>
-      <c r="K68" s="6" t="s">
+      <c r="L68" s="8" t="s">
         <v>473</v>
       </c>
-      <c r="L68" s="6" t="s">
-        <v>474</v>
-      </c>
-      <c r="M68" s="2"/>
-      <c r="N68" s="3"/>
+      <c r="M68" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="N68" s="3" t="s">
+        <v>290</v>
+      </c>
       <c r="O68" s="6"/>
     </row>
-    <row r="69" spans="1:15" ht="45">
+    <row r="69" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A69" s="2"/>
       <c r="B69" s="4">
         <v>43441</v>
@@ -4211,10 +4218,10 @@
         <v>442</v>
       </c>
       <c r="D69" s="18" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="E69" s="19" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="F69" s="18" t="s">
         <v>27</v>
@@ -4223,19 +4230,19 @@
       <c r="H69" s="18"/>
       <c r="I69" s="18"/>
       <c r="J69" s="19" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="K69" s="6" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="L69" s="6" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="M69" s="3"/>
       <c r="N69" s="3"/>
       <c r="O69" s="6"/>
     </row>
-    <row r="70" spans="1:15" ht="45">
+    <row r="70" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A70" s="2"/>
       <c r="B70" s="4">
         <v>43441</v>
@@ -4244,10 +4251,10 @@
         <v>56</v>
       </c>
       <c r="D70" s="18" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="E70" s="19" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="F70" s="18" t="s">
         <v>27</v>
@@ -4256,44 +4263,44 @@
       <c r="H70" s="18"/>
       <c r="I70" s="18"/>
       <c r="J70" s="18" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
       <c r="K70" s="6" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="L70" s="6" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="M70" s="2"/>
       <c r="N70" s="3"/>
       <c r="O70" s="6"/>
     </row>
-    <row r="71" spans="1:15" ht="45.75" customHeight="1">
+    <row r="71" spans="1:15" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="2"/>
-      <c r="B71" s="4">
+      <c r="B71" s="28">
         <v>43441</v>
       </c>
-      <c r="C71" s="19" t="s">
+      <c r="C71" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="D71" s="18" t="s">
-        <v>452</v>
-      </c>
-      <c r="E71" s="19" t="s">
+      <c r="D71" s="29" t="s">
+        <v>451</v>
+      </c>
+      <c r="E71" s="26" t="s">
+        <v>482</v>
+      </c>
+      <c r="F71" s="29"/>
+      <c r="G71" s="29"/>
+      <c r="H71" s="29"/>
+      <c r="I71" s="29"/>
+      <c r="J71" s="26" t="s">
+        <v>519</v>
+      </c>
+      <c r="K71" s="6" t="s">
+        <v>483</v>
+      </c>
+      <c r="L71" s="8" t="s">
         <v>484</v>
-      </c>
-      <c r="F71" s="18"/>
-      <c r="G71" s="18"/>
-      <c r="H71" s="18"/>
-      <c r="I71" s="18"/>
-      <c r="J71" s="19" t="s">
-        <v>486</v>
-      </c>
-      <c r="K71" s="6" t="s">
-        <v>485</v>
-      </c>
-      <c r="L71" s="6" t="s">
-        <v>487</v>
       </c>
       <c r="M71" s="3" t="s">
         <v>13</v>
@@ -4303,19 +4310,19 @@
       </c>
       <c r="O71" s="6"/>
     </row>
-    <row r="72" spans="1:15" ht="45">
+    <row r="72" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A72" s="2"/>
       <c r="B72" s="4">
         <v>43441</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="D72" s="2" t="s">
         <v>279</v>
       </c>
       <c r="E72" s="6" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
       <c r="F72" s="2" t="s">
         <v>27</v>
@@ -4323,67 +4330,67 @@
       <c r="G72" s="2"/>
       <c r="H72" s="2"/>
       <c r="I72" s="2"/>
-      <c r="J72" s="2" t="s">
+      <c r="J72" s="26" t="s">
+        <v>519</v>
+      </c>
+      <c r="K72" s="6" t="s">
+        <v>492</v>
+      </c>
+      <c r="L72" s="6" t="s">
+        <v>487</v>
+      </c>
+      <c r="M72" s="8" t="s">
         <v>489</v>
-      </c>
-      <c r="K72" s="6" t="s">
-        <v>496</v>
-      </c>
-      <c r="L72" s="6" t="s">
-        <v>491</v>
-      </c>
-      <c r="M72" s="8" t="s">
-        <v>493</v>
       </c>
       <c r="N72" s="3" t="s">
         <v>272</v>
       </c>
       <c r="O72" s="6"/>
     </row>
-    <row r="73" spans="1:15" ht="45">
+    <row r="73" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A73" s="2"/>
       <c r="B73" s="4">
         <v>43441</v>
       </c>
       <c r="C73" s="6" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="D73" s="2" t="s">
         <v>279</v>
       </c>
       <c r="E73" s="6" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="F73" s="2"/>
       <c r="G73" s="2"/>
       <c r="H73" s="2"/>
       <c r="I73" s="2"/>
       <c r="J73" s="2" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="K73" s="6" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
       <c r="L73" s="6" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="M73" s="2"/>
       <c r="N73" s="3"/>
       <c r="O73" s="6"/>
     </row>
-    <row r="74" spans="1:15" ht="30">
+    <row r="74" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A74" s="2"/>
       <c r="B74" s="4">
         <v>43441</v>
       </c>
       <c r="C74" s="6" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
       <c r="D74" s="2" t="s">
         <v>279</v>
       </c>
       <c r="E74" s="6" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="F74" s="2" t="s">
         <v>31</v>
@@ -4393,57 +4400,57 @@
       <c r="I74" s="2"/>
       <c r="J74" s="2"/>
       <c r="K74" s="6" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="L74" s="6"/>
       <c r="M74" s="2"/>
       <c r="N74" s="3"/>
       <c r="O74" s="6"/>
     </row>
-    <row r="75" spans="1:15" ht="48" customHeight="1">
+    <row r="75" spans="1:15" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="2"/>
       <c r="B75" s="4">
         <v>43441</v>
       </c>
       <c r="C75" s="19" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="D75" s="18" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="E75" s="19" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="F75" s="18"/>
       <c r="G75" s="18"/>
       <c r="H75" s="18"/>
       <c r="I75" s="18"/>
       <c r="J75" s="18" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
       <c r="K75" s="6" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
       <c r="L75" s="6" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="M75" s="2"/>
       <c r="N75" s="3"/>
       <c r="O75" s="6"/>
     </row>
-    <row r="76" spans="1:15" ht="41.25" customHeight="1">
+    <row r="76" spans="1:15" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="2"/>
       <c r="B76" s="4">
         <v>43441</v>
       </c>
       <c r="C76" s="6" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="E76" s="6" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="F76" s="2" t="s">
         <v>27</v>
@@ -4452,29 +4459,29 @@
       <c r="H76" s="2"/>
       <c r="I76" s="2"/>
       <c r="J76" s="6" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
       <c r="K76" s="6"/>
       <c r="L76" s="6" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
       <c r="M76" s="2"/>
       <c r="N76" s="3"/>
       <c r="O76" s="6"/>
     </row>
-    <row r="77" spans="1:15" ht="30">
+    <row r="77" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A77" s="2"/>
       <c r="B77" s="4">
         <v>43441</v>
       </c>
       <c r="C77" s="6" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="E77" s="6" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="F77" s="2" t="s">
         <v>27</v>
@@ -4484,28 +4491,28 @@
       <c r="I77" s="2"/>
       <c r="J77" s="2"/>
       <c r="K77" s="6" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
       <c r="L77" s="6" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
       <c r="M77" s="2"/>
       <c r="N77" s="3"/>
       <c r="O77" s="6"/>
     </row>
-    <row r="78" spans="1:15" ht="30">
+    <row r="78" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A78" s="2"/>
       <c r="B78" s="4">
         <v>43441</v>
       </c>
       <c r="C78" s="6" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="E78" s="6" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="F78" s="2" t="s">
         <v>27</v>
@@ -4515,47 +4522,47 @@
       <c r="I78" s="2"/>
       <c r="J78" s="2"/>
       <c r="K78" s="6" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="L78" s="6" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
       <c r="M78" s="2"/>
       <c r="N78" s="3"/>
       <c r="O78" s="6"/>
     </row>
-    <row r="79" spans="1:15" ht="54" customHeight="1">
+    <row r="79" spans="1:15" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="2"/>
       <c r="B79" s="4">
         <v>43441</v>
       </c>
       <c r="C79" s="19" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
       <c r="D79" s="18" t="s">
         <v>33</v>
       </c>
       <c r="E79" s="19" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
       <c r="F79" s="18"/>
       <c r="G79" s="18"/>
       <c r="H79" s="18"/>
       <c r="I79" s="18"/>
       <c r="J79" s="18" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
       <c r="K79" s="6" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
       <c r="L79" s="6" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
       <c r="M79" s="2"/>
       <c r="N79" s="3"/>
       <c r="O79" s="6"/>
     </row>
-    <row r="80" spans="1:15">
+    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A80" s="2"/>
       <c r="B80" s="4"/>
       <c r="C80" s="6"/>
@@ -4572,7 +4579,7 @@
       <c r="N80" s="3"/>
       <c r="O80" s="6"/>
     </row>
-    <row r="81" spans="1:15">
+    <row r="81" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A81" s="2"/>
       <c r="B81" s="4"/>
       <c r="C81" s="6"/>
@@ -4589,7 +4596,7 @@
       <c r="N81" s="3"/>
       <c r="O81" s="6"/>
     </row>
-    <row r="82" spans="1:15">
+    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A82" s="2"/>
       <c r="B82" s="4"/>
       <c r="C82" s="6"/>
@@ -4606,7 +4613,7 @@
       <c r="N82" s="3"/>
       <c r="O82" s="6"/>
     </row>
-    <row r="83" spans="1:15">
+    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A83" s="2"/>
       <c r="B83" s="4"/>
       <c r="C83" s="6"/>
@@ -4623,7 +4630,7 @@
       <c r="N83" s="3"/>
       <c r="O83" s="6"/>
     </row>
-    <row r="84" spans="1:15">
+    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A84" s="2"/>
       <c r="B84" s="4"/>
       <c r="C84" s="6"/>
@@ -4640,7 +4647,7 @@
       <c r="N84" s="3"/>
       <c r="O84" s="6"/>
     </row>
-    <row r="85" spans="1:15">
+    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A85" s="2"/>
       <c r="B85" s="4"/>
       <c r="C85" s="6"/>
@@ -4657,7 +4664,7 @@
       <c r="N85" s="3"/>
       <c r="O85" s="6"/>
     </row>
-    <row r="86" spans="1:15">
+    <row r="86" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A86" s="2"/>
       <c r="B86" s="4"/>
       <c r="C86" s="6"/>
@@ -4674,7 +4681,7 @@
       <c r="N86" s="3"/>
       <c r="O86" s="6"/>
     </row>
-    <row r="87" spans="1:15">
+    <row r="87" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A87" s="2"/>
       <c r="B87" s="4"/>
       <c r="C87" s="6"/>
@@ -4691,7 +4698,7 @@
       <c r="N87" s="3"/>
       <c r="O87" s="6"/>
     </row>
-    <row r="88" spans="1:15">
+    <row r="88" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A88" s="2"/>
       <c r="B88" s="4"/>
       <c r="C88" s="6"/>
@@ -4708,7 +4715,7 @@
       <c r="N88" s="3"/>
       <c r="O88" s="6"/>
     </row>
-    <row r="89" spans="1:15">
+    <row r="89" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A89" s="2"/>
       <c r="B89" s="4"/>
       <c r="C89" s="6"/>
@@ -4725,7 +4732,7 @@
       <c r="N89" s="3"/>
       <c r="O89" s="6"/>
     </row>
-    <row r="90" spans="1:15">
+    <row r="90" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A90" s="2"/>
       <c r="B90" s="4"/>
       <c r="C90" s="6"/>
@@ -4742,7 +4749,7 @@
       <c r="N90" s="3"/>
       <c r="O90" s="6"/>
     </row>
-    <row r="91" spans="1:15">
+    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A91" s="2"/>
       <c r="B91" s="4"/>
       <c r="C91" s="6"/>
@@ -4759,7 +4766,7 @@
       <c r="N91" s="3"/>
       <c r="O91" s="6"/>
     </row>
-    <row r="92" spans="1:15">
+    <row r="92" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A92" s="2"/>
       <c r="B92" s="4"/>
       <c r="C92" s="6"/>
@@ -4776,7 +4783,7 @@
       <c r="N92" s="3"/>
       <c r="O92" s="6"/>
     </row>
-    <row r="93" spans="1:15">
+    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A93" s="2"/>
       <c r="B93" s="4"/>
       <c r="C93" s="6"/>
@@ -4795,12 +4802,12 @@
       <c r="N93" s="3"/>
       <c r="O93" s="6"/>
     </row>
-    <row r="94" spans="1:15">
+    <row r="94" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A94" s="2"/>
       <c r="B94" s="4"/>
       <c r="C94" s="6"/>
       <c r="D94" s="2" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="E94" s="6"/>
       <c r="F94" s="2"/>
@@ -4814,7 +4821,7 @@
       <c r="N94" s="3"/>
       <c r="O94" s="6"/>
     </row>
-    <row r="95" spans="1:15">
+    <row r="95" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A95" s="2"/>
       <c r="B95" s="4"/>
       <c r="C95" s="6"/>
@@ -4831,7 +4838,7 @@
       <c r="N95" s="3"/>
       <c r="O95" s="6"/>
     </row>
-    <row r="96" spans="1:15">
+    <row r="96" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A96" s="2"/>
       <c r="B96" s="4"/>
       <c r="C96" s="6"/>
@@ -4848,7 +4855,7 @@
       <c r="N96" s="3"/>
       <c r="O96" s="6"/>
     </row>
-    <row r="97" spans="1:15">
+    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A97" s="2"/>
       <c r="B97" s="4"/>
       <c r="C97" s="6"/>
@@ -4865,7 +4872,7 @@
       <c r="N97" s="3"/>
       <c r="O97" s="6"/>
     </row>
-    <row r="98" spans="1:15">
+    <row r="98" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A98" s="2"/>
       <c r="B98" s="4"/>
       <c r="C98" s="6"/>
@@ -4882,7 +4889,7 @@
       <c r="N98" s="3"/>
       <c r="O98" s="6"/>
     </row>
-    <row r="99" spans="1:15">
+    <row r="99" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A99" s="2"/>
       <c r="B99" s="4"/>
       <c r="C99" s="6"/>
@@ -4899,7 +4906,7 @@
       <c r="N99" s="3"/>
       <c r="O99" s="6"/>
     </row>
-    <row r="100" spans="1:15">
+    <row r="100" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A100" s="2"/>
       <c r="B100" s="4"/>
       <c r="C100" s="6"/>
@@ -4916,7 +4923,7 @@
       <c r="N100" s="3"/>
       <c r="O100" s="6"/>
     </row>
-    <row r="101" spans="1:15">
+    <row r="101" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A101" s="2"/>
       <c r="B101" s="4"/>
       <c r="C101" s="6"/>
@@ -4933,7 +4940,7 @@
       <c r="N101" s="3"/>
       <c r="O101" s="6"/>
     </row>
-    <row r="102" spans="1:15">
+    <row r="102" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A102" s="2"/>
       <c r="B102" s="4"/>
       <c r="C102" s="6"/>
@@ -4950,7 +4957,7 @@
       <c r="N102" s="3"/>
       <c r="O102" s="6"/>
     </row>
-    <row r="103" spans="1:15">
+    <row r="103" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A103" s="2"/>
       <c r="B103" s="4"/>
       <c r="C103" s="6"/>
@@ -4967,7 +4974,7 @@
       <c r="N103" s="3"/>
       <c r="O103" s="6"/>
     </row>
-    <row r="104" spans="1:15">
+    <row r="104" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A104" s="2"/>
       <c r="B104" s="4"/>
       <c r="C104" s="6"/>
@@ -4984,7 +4991,7 @@
       <c r="N104" s="3"/>
       <c r="O104" s="6"/>
     </row>
-    <row r="105" spans="1:15">
+    <row r="105" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A105" s="2"/>
       <c r="B105" s="4"/>
       <c r="C105" s="6"/>
@@ -5001,7 +5008,7 @@
       <c r="N105" s="3"/>
       <c r="O105" s="6"/>
     </row>
-    <row r="106" spans="1:15">
+    <row r="106" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A106" s="2"/>
       <c r="B106" s="4"/>
       <c r="C106" s="6"/>
@@ -5018,7 +5025,7 @@
       <c r="N106" s="3"/>
       <c r="O106" s="6"/>
     </row>
-    <row r="107" spans="1:15">
+    <row r="107" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A107" s="2"/>
       <c r="B107" s="4"/>
       <c r="C107" s="6"/>
@@ -5035,7 +5042,7 @@
       <c r="N107" s="3"/>
       <c r="O107" s="6"/>
     </row>
-    <row r="108" spans="1:15">
+    <row r="108" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A108" s="2"/>
       <c r="B108" s="4"/>
       <c r="C108" s="6"/>
@@ -5052,7 +5059,7 @@
       <c r="N108" s="3"/>
       <c r="O108" s="6"/>
     </row>
-    <row r="109" spans="1:15">
+    <row r="109" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A109" s="2"/>
       <c r="B109" s="4"/>
       <c r="C109" s="6"/>
@@ -5069,7 +5076,7 @@
       <c r="N109" s="3"/>
       <c r="O109" s="6"/>
     </row>
-    <row r="110" spans="1:15" ht="409.6">
+    <row r="110" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A110" s="2"/>
       <c r="B110" s="4"/>
       <c r="C110" s="6"/>
@@ -5086,7 +5093,7 @@
       <c r="N110" s="3"/>
       <c r="O110" s="6"/>
     </row>
-    <row r="111" spans="1:15" ht="409.6">
+    <row r="111" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A111" s="2"/>
       <c r="B111" s="4"/>
       <c r="C111" s="6"/>
@@ -5103,7 +5110,7 @@
       <c r="N111" s="3"/>
       <c r="O111" s="6"/>
     </row>
-    <row r="112" spans="1:15" ht="409.6">
+    <row r="112" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A112" s="2"/>
       <c r="B112" s="4"/>
       <c r="C112" s="6"/>
@@ -5120,7 +5127,7 @@
       <c r="N112" s="3"/>
       <c r="O112" s="6"/>
     </row>
-    <row r="113" spans="1:15">
+    <row r="113" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A113" s="2"/>
       <c r="B113" s="4"/>
       <c r="C113" s="6"/>
@@ -5137,7 +5144,7 @@
       <c r="N113" s="3"/>
       <c r="O113" s="6"/>
     </row>
-    <row r="114" spans="1:15" ht="409.6">
+    <row r="114" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A114" s="2"/>
       <c r="B114" s="4"/>
       <c r="C114" s="6"/>
@@ -5154,7 +5161,7 @@
       <c r="N114" s="3"/>
       <c r="O114" s="6"/>
     </row>
-    <row r="115" spans="1:15" ht="409.6">
+    <row r="115" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A115" s="2"/>
       <c r="B115" s="4"/>
       <c r="C115" s="6"/>
@@ -5171,7 +5178,7 @@
       <c r="N115" s="3"/>
       <c r="O115" s="6"/>
     </row>
-    <row r="116" spans="1:15" ht="409.6">
+    <row r="116" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A116" s="2"/>
       <c r="B116" s="4"/>
       <c r="C116" s="6"/>
@@ -5188,7 +5195,7 @@
       <c r="N116" s="3"/>
       <c r="O116" s="6"/>
     </row>
-    <row r="117" spans="1:15" ht="409.6">
+    <row r="117" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A117" s="2"/>
       <c r="B117" s="4"/>
       <c r="C117" s="6"/>
@@ -5205,7 +5212,7 @@
       <c r="N117" s="3"/>
       <c r="O117" s="6"/>
     </row>
-    <row r="118" spans="1:15">
+    <row r="118" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A118" s="2"/>
       <c r="B118" s="4"/>
       <c r="C118" s="6"/>
@@ -5222,7 +5229,7 @@
       <c r="N118" s="3"/>
       <c r="O118" s="6"/>
     </row>
-    <row r="119" spans="1:15">
+    <row r="119" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A119" s="2"/>
       <c r="B119" s="4"/>
       <c r="C119" s="6"/>
@@ -5240,75 +5247,79 @@
       <c r="O119" s="6"/>
     </row>
   </sheetData>
-  <autoFilter ref="C1:C119"/>
+  <autoFilter ref="C1:C119" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <hyperlinks>
-    <hyperlink ref="M2" r:id="rId1"/>
-    <hyperlink ref="N2" r:id="rId2"/>
-    <hyperlink ref="J4" r:id="rId3" tooltip="View this job description" display="https://autodesk.taleo.net/careersection/careersection/candidateacquisition/flow.jsf"/>
-    <hyperlink ref="L9" r:id="rId4"/>
-    <hyperlink ref="M14" r:id="rId5"/>
-    <hyperlink ref="N14" r:id="rId6"/>
-    <hyperlink ref="N20" r:id="rId7"/>
-    <hyperlink ref="N21" r:id="rId8"/>
-    <hyperlink ref="M21" r:id="rId9"/>
-    <hyperlink ref="N23" r:id="rId10"/>
-    <hyperlink ref="M23" r:id="rId11"/>
-    <hyperlink ref="N25" r:id="rId12"/>
-    <hyperlink ref="N28" r:id="rId13"/>
-    <hyperlink ref="L28" r:id="rId14" display="https://career8.successfactors.com/portalcareer?_s.crb=kNBYkSysisIRZTdxfVciJ8DJuxM%253d"/>
-    <hyperlink ref="N31" r:id="rId15"/>
-    <hyperlink ref="M32" r:id="rId16"/>
-    <hyperlink ref="N32" r:id="rId17"/>
-    <hyperlink ref="N24" r:id="rId18"/>
-    <hyperlink ref="L26" r:id="rId19"/>
-    <hyperlink ref="M36" r:id="rId20"/>
-    <hyperlink ref="N36" r:id="rId21"/>
-    <hyperlink ref="M41" r:id="rId22"/>
-    <hyperlink ref="N41" r:id="rId23"/>
-    <hyperlink ref="K41" r:id="rId24"/>
-    <hyperlink ref="L41" display="https://garmin.taleo.net/careersection/iam/accessmanagement/login.jsf?redirectionURI=https%3A%2F%2Fgarmin.taleo.net%2Fcareersection%2F2012_garmin_exp_tech%2Fjobsearch.ftl%3Fftlcompclass%3DLoginComponent&amp;TARGET=https%3A%2F%2Fgarmin.taleo.net%2Fcareersectio"/>
-    <hyperlink ref="M46" r:id="rId25"/>
-    <hyperlink ref="N46" r:id="rId26"/>
-    <hyperlink ref="M47" r:id="rId27"/>
-    <hyperlink ref="N47" r:id="rId28"/>
-    <hyperlink ref="L50" r:id="rId29"/>
-    <hyperlink ref="L51" r:id="rId30"/>
-    <hyperlink ref="M54" r:id="rId31"/>
-    <hyperlink ref="N54" r:id="rId32"/>
-    <hyperlink ref="M55" r:id="rId33"/>
-    <hyperlink ref="N55" r:id="rId34"/>
-    <hyperlink ref="M57" r:id="rId35"/>
-    <hyperlink ref="N57" r:id="rId36"/>
-    <hyperlink ref="M62" r:id="rId37"/>
-    <hyperlink ref="N62" r:id="rId38"/>
-    <hyperlink ref="L62" r:id="rId39"/>
-    <hyperlink ref="M67" r:id="rId40"/>
-    <hyperlink ref="N67" r:id="rId41"/>
-    <hyperlink ref="M71" r:id="rId42"/>
-    <hyperlink ref="N71" r:id="rId43"/>
-    <hyperlink ref="M72" r:id="rId44" display="sarath.sund@gmail.com"/>
-    <hyperlink ref="N72" r:id="rId45"/>
+    <hyperlink ref="M2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="N2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="J4" r:id="rId3" tooltip="View this job description" display="https://autodesk.taleo.net/careersection/careersection/candidateacquisition/flow.jsf" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="L9" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="M14" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="N14" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="N20" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="N21" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="M21" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="N23" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="M23" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="N25" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="N28" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="L28" r:id="rId14" display="https://career8.successfactors.com/portalcareer?_s.crb=kNBYkSysisIRZTdxfVciJ8DJuxM%253d" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="N31" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="M32" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="N32" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="N24" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="L26" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="M36" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="N36" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="M41" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="N41" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="K41" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="L41" display="https://garmin.taleo.net/careersection/iam/accessmanagement/login.jsf?redirectionURI=https%3A%2F%2Fgarmin.taleo.net%2Fcareersection%2F2012_garmin_exp_tech%2Fjobsearch.ftl%3Fftlcompclass%3DLoginComponent&amp;TARGET=https%3A%2F%2Fgarmin.taleo.net%2Fcareersectio" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="M46" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="N46" r:id="rId26" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="M47" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="N47" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="L50" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="L51" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="M54" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="N54" r:id="rId32" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="M55" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="N55" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="M57" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="N57" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="M62" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="N62" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="L62" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="M67" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="N67" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="M71" r:id="rId42" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="N71" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="M72" r:id="rId44" display="sarath.sund@gmail.com" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="N72" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="L71" r:id="rId46" location="jobDetails=410516_5185" xr:uid="{6DA754AB-8E1A-404C-A18E-1675FF87B213}"/>
+    <hyperlink ref="L68" r:id="rId47" xr:uid="{4DCC1BC6-DA4A-44A5-A237-9DE01F1647C3}"/>
+    <hyperlink ref="M68" r:id="rId48" xr:uid="{D18D236A-14AD-436B-B1C2-FE8611B9E569}"/>
+    <hyperlink ref="N68" r:id="rId49" xr:uid="{D3A739E5-9A28-4728-B37E-624F5E59207E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId46"/>
+  <pageSetup orientation="portrait" r:id="rId50"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="D3:F22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="23" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="4:6">
+    <row r="3" spans="4:6" x14ac:dyDescent="0.25">
       <c r="E3" s="9" t="s">
         <v>60</v>
       </c>
@@ -5316,7 +5327,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="4:6">
+    <row r="4" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D4">
         <v>1</v>
       </c>
@@ -5327,7 +5338,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="4:6">
+    <row r="5" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D5">
         <v>2</v>
       </c>
@@ -5338,7 +5349,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="4:6">
+    <row r="6" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D6">
         <v>3</v>
       </c>
@@ -5349,7 +5360,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="4:6">
+    <row r="7" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D7">
         <v>4</v>
       </c>
@@ -5357,7 +5368,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="4:6">
+    <row r="8" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D8">
         <v>5</v>
       </c>
@@ -5365,7 +5376,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="4:6">
+    <row r="9" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D9">
         <v>6</v>
       </c>
@@ -5373,7 +5384,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="4:6">
+    <row r="10" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D10">
         <v>7</v>
       </c>
@@ -5381,7 +5392,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="4:6">
+    <row r="11" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D11">
         <v>8</v>
       </c>
@@ -5389,7 +5400,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="4:6">
+    <row r="12" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D12">
         <v>9</v>
       </c>
@@ -5397,7 +5408,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="4:6">
+    <row r="13" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D13">
         <v>10</v>
       </c>
@@ -5405,7 +5416,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="14" spans="4:6">
+    <row r="14" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D14">
         <v>11</v>
       </c>
@@ -5413,7 +5424,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="4:6">
+    <row r="15" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D15">
         <v>12</v>
       </c>
@@ -5421,7 +5432,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="4:6">
+    <row r="16" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D16">
         <v>13</v>
       </c>
@@ -5429,7 +5440,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="17" spans="4:5">
+    <row r="17" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D17">
         <v>14</v>
       </c>
@@ -5437,7 +5448,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="18" spans="4:5">
+    <row r="18" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D18">
         <v>15</v>
       </c>
@@ -5445,7 +5456,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="19" spans="4:5">
+    <row r="19" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D19">
         <v>16</v>
       </c>
@@ -5453,7 +5464,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="20" spans="4:5">
+    <row r="20" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D20">
         <v>17</v>
       </c>
@@ -5461,7 +5472,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="21" spans="4:5">
+    <row r="21" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D21">
         <v>18</v>
       </c>
@@ -5469,7 +5480,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="22" spans="4:5">
+    <row r="22" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D22">
         <v>19</v>
       </c>
@@ -5484,19 +5495,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="E1:G86"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="6" max="7" width="48.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="5:7" ht="15.75" thickBot="1">
+    <row r="1" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E1" s="10" t="s">
         <v>0</v>
       </c>
@@ -5507,7 +5518,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="5:7" ht="16.5" thickTop="1" thickBot="1">
+    <row r="2" spans="5:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E2">
         <v>1</v>
       </c>
@@ -5518,7 +5529,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="5:7" ht="15.75" thickBot="1">
+    <row r="3" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E3">
         <v>2</v>
       </c>
@@ -5529,7 +5540,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="5:7" ht="15.75" thickBot="1">
+    <row r="4" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E4">
         <v>3</v>
       </c>
@@ -5540,7 +5551,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="5" spans="5:7" ht="15.75" thickBot="1">
+    <row r="5" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E5">
         <v>4</v>
       </c>
@@ -5551,7 +5562,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="5:7" ht="15.75" thickBot="1">
+    <row r="6" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E6">
         <v>5</v>
       </c>
@@ -5562,7 +5573,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="5:7" ht="15.75" thickBot="1">
+    <row r="7" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E7">
         <v>6</v>
       </c>
@@ -5573,7 +5584,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="8" spans="5:7" ht="15.75" thickBot="1">
+    <row r="8" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E8">
         <v>7</v>
       </c>
@@ -5584,7 +5595,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="9" spans="5:7" ht="15.75" thickBot="1">
+    <row r="9" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E9">
         <v>8</v>
       </c>
@@ -5595,7 +5606,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="10" spans="5:7" ht="15.75" thickBot="1">
+    <row r="10" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E10">
         <v>9</v>
       </c>
@@ -5606,7 +5617,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="11" spans="5:7" ht="15.75" thickBot="1">
+    <row r="11" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E11">
         <v>10</v>
       </c>
@@ -5617,7 +5628,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="12" spans="5:7" ht="15.75" thickBot="1">
+    <row r="12" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E12">
         <v>11</v>
       </c>
@@ -5628,7 +5639,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="13" spans="5:7" ht="15.75" thickBot="1">
+    <row r="13" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E13">
         <v>12</v>
       </c>
@@ -5639,7 +5650,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="14" spans="5:7" ht="15.75" thickBot="1">
+    <row r="14" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E14">
         <v>13</v>
       </c>
@@ -5650,7 +5661,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="15" spans="5:7" ht="15.75" thickBot="1">
+    <row r="15" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E15">
         <v>14</v>
       </c>
@@ -5661,7 +5672,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="16" spans="5:7" ht="15.75" thickBot="1">
+    <row r="16" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E16">
         <v>15</v>
       </c>
@@ -5672,7 +5683,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="17" spans="5:7" ht="15.75" thickBot="1">
+    <row r="17" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E17">
         <v>16</v>
       </c>
@@ -5683,7 +5694,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="18" spans="5:7" ht="15.75" thickBot="1">
+    <row r="18" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E18">
         <v>17</v>
       </c>
@@ -5694,7 +5705,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="19" spans="5:7" ht="15.75" thickBot="1">
+    <row r="19" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E19">
         <v>18</v>
       </c>
@@ -5705,7 +5716,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="20" spans="5:7" ht="15.75" thickBot="1">
+    <row r="20" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E20">
         <v>19</v>
       </c>
@@ -5716,7 +5727,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="21" spans="5:7" ht="15.75" thickBot="1">
+    <row r="21" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E21">
         <v>20</v>
       </c>
@@ -5727,7 +5738,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="22" spans="5:7" ht="15.75" thickBot="1">
+    <row r="22" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E22">
         <v>21</v>
       </c>
@@ -5738,7 +5749,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="23" spans="5:7" ht="15.75" thickBot="1">
+    <row r="23" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E23">
         <v>22</v>
       </c>
@@ -5749,7 +5760,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="24" spans="5:7" ht="15.75" thickBot="1">
+    <row r="24" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E24">
         <v>23</v>
       </c>
@@ -5760,7 +5771,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="25" spans="5:7" ht="15.75" thickBot="1">
+    <row r="25" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E25">
         <v>24</v>
       </c>
@@ -5771,7 +5782,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="26" spans="5:7" ht="15.75" thickBot="1">
+    <row r="26" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E26">
         <v>25</v>
       </c>
@@ -5782,7 +5793,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="27" spans="5:7" ht="15.75" thickBot="1">
+    <row r="27" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E27">
         <v>26</v>
       </c>
@@ -5793,7 +5804,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="28" spans="5:7" ht="15.75" thickBot="1">
+    <row r="28" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E28">
         <v>27</v>
       </c>
@@ -5804,7 +5815,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="29" spans="5:7" ht="15.75" thickBot="1">
+    <row r="29" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E29">
         <v>28</v>
       </c>
@@ -5815,7 +5826,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="30" spans="5:7" ht="15.75" thickBot="1">
+    <row r="30" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E30">
         <v>29</v>
       </c>
@@ -5826,7 +5837,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="31" spans="5:7" ht="15.75" thickBot="1">
+    <row r="31" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E31">
         <v>30</v>
       </c>
@@ -5837,7 +5848,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="32" spans="5:7" ht="15.75" thickBot="1">
+    <row r="32" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E32">
         <v>31</v>
       </c>
@@ -5848,7 +5859,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="33" spans="5:7" ht="15.75" thickBot="1">
+    <row r="33" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E33">
         <v>32</v>
       </c>
@@ -5859,7 +5870,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="34" spans="5:7" ht="15.75" thickBot="1">
+    <row r="34" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E34">
         <v>33</v>
       </c>
@@ -5870,7 +5881,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="35" spans="5:7" ht="15.75" thickBot="1">
+    <row r="35" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E35">
         <v>34</v>
       </c>
@@ -5881,7 +5892,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="36" spans="5:7" ht="15.75" thickBot="1">
+    <row r="36" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E36">
         <v>35</v>
       </c>
@@ -5892,7 +5903,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="37" spans="5:7" ht="15.75" thickBot="1">
+    <row r="37" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E37">
         <v>36</v>
       </c>
@@ -5903,7 +5914,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="38" spans="5:7" ht="15.75" thickBot="1">
+    <row r="38" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E38">
         <v>37</v>
       </c>
@@ -5914,7 +5925,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="39" spans="5:7" ht="15.75" thickBot="1">
+    <row r="39" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E39">
         <v>38</v>
       </c>
@@ -5925,7 +5936,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="40" spans="5:7" ht="15.75" thickBot="1">
+    <row r="40" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E40">
         <v>39</v>
       </c>
@@ -5936,7 +5947,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="41" spans="5:7" ht="15.75" thickBot="1">
+    <row r="41" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E41">
         <v>40</v>
       </c>
@@ -5947,7 +5958,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="42" spans="5:7" ht="15.75" thickBot="1">
+    <row r="42" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E42">
         <v>41</v>
       </c>
@@ -5958,7 +5969,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="43" spans="5:7" ht="15.75" thickBot="1">
+    <row r="43" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E43">
         <v>42</v>
       </c>
@@ -5969,7 +5980,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="44" spans="5:7" ht="15.75" thickBot="1">
+    <row r="44" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E44">
         <v>43</v>
       </c>
@@ -5980,7 +5991,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="45" spans="5:7" ht="15.75" thickBot="1">
+    <row r="45" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E45">
         <v>44</v>
       </c>
@@ -5991,7 +6002,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="46" spans="5:7" ht="15.75" thickBot="1">
+    <row r="46" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E46">
         <v>45</v>
       </c>
@@ -6002,7 +6013,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="47" spans="5:7" ht="15.75" thickBot="1">
+    <row r="47" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E47">
         <v>46</v>
       </c>
@@ -6013,7 +6024,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="48" spans="5:7" ht="15.75" thickBot="1">
+    <row r="48" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E48">
         <v>47</v>
       </c>
@@ -6024,7 +6035,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="49" spans="5:7" ht="15.75" thickBot="1">
+    <row r="49" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E49">
         <v>48</v>
       </c>
@@ -6035,7 +6046,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="50" spans="5:7" ht="15.75" thickBot="1">
+    <row r="50" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E50">
         <v>49</v>
       </c>
@@ -6046,7 +6057,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="51" spans="5:7" ht="15.75" thickBot="1">
+    <row r="51" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E51">
         <v>50</v>
       </c>
@@ -6057,7 +6068,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="52" spans="5:7" ht="15.75" thickBot="1">
+    <row r="52" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E52">
         <v>51</v>
       </c>
@@ -6068,7 +6079,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="53" spans="5:7" ht="15.75" thickBot="1">
+    <row r="53" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E53">
         <v>52</v>
       </c>
@@ -6079,7 +6090,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="54" spans="5:7" ht="15.75" thickBot="1">
+    <row r="54" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E54">
         <v>53</v>
       </c>
@@ -6090,7 +6101,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="55" spans="5:7" ht="15.75" thickBot="1">
+    <row r="55" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E55">
         <v>54</v>
       </c>
@@ -6101,7 +6112,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="56" spans="5:7" ht="15.75" thickBot="1">
+    <row r="56" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E56">
         <v>55</v>
       </c>
@@ -6112,7 +6123,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="57" spans="5:7" ht="15.75" thickBot="1">
+    <row r="57" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E57">
         <v>56</v>
       </c>
@@ -6123,7 +6134,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="58" spans="5:7" ht="15.75" thickBot="1">
+    <row r="58" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E58">
         <v>57</v>
       </c>
@@ -6134,7 +6145,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="59" spans="5:7" ht="15.75" thickBot="1">
+    <row r="59" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E59">
         <v>58</v>
       </c>
@@ -6145,7 +6156,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="60" spans="5:7" ht="15.75" thickBot="1">
+    <row r="60" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E60">
         <v>59</v>
       </c>
@@ -6156,7 +6167,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="61" spans="5:7" ht="15.75" thickBot="1">
+    <row r="61" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E61">
         <v>60</v>
       </c>
@@ -6167,7 +6178,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="62" spans="5:7" ht="15.75" thickBot="1">
+    <row r="62" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E62">
         <v>61</v>
       </c>
@@ -6178,7 +6189,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="63" spans="5:7" ht="15.75" thickBot="1">
+    <row r="63" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E63">
         <v>62</v>
       </c>
@@ -6189,7 +6200,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="64" spans="5:7" ht="15.75" thickBot="1">
+    <row r="64" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E64">
         <v>63</v>
       </c>
@@ -6200,7 +6211,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="65" spans="5:7" ht="15.75" thickBot="1">
+    <row r="65" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E65">
         <v>64</v>
       </c>
@@ -6211,7 +6222,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="66" spans="5:7" ht="15.75" thickBot="1">
+    <row r="66" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E66">
         <v>65</v>
       </c>
@@ -6222,7 +6233,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="67" spans="5:7" ht="15.75" thickBot="1">
+    <row r="67" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E67">
         <v>66</v>
       </c>
@@ -6233,7 +6244,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="68" spans="5:7" ht="15.75" thickBot="1">
+    <row r="68" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E68">
         <v>67</v>
       </c>
@@ -6244,7 +6255,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="69" spans="5:7" ht="15.75" thickBot="1">
+    <row r="69" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E69">
         <v>68</v>
       </c>
@@ -6255,7 +6266,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="70" spans="5:7" ht="15.75" thickBot="1">
+    <row r="70" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E70">
         <v>69</v>
       </c>
@@ -6266,7 +6277,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="71" spans="5:7" ht="15.75" thickBot="1">
+    <row r="71" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E71">
         <v>70</v>
       </c>
@@ -6277,7 +6288,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="72" spans="5:7" ht="15.75" thickBot="1">
+    <row r="72" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E72">
         <v>71</v>
       </c>
@@ -6288,7 +6299,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="73" spans="5:7" ht="15.75" thickBot="1">
+    <row r="73" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E73">
         <v>72</v>
       </c>
@@ -6299,7 +6310,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="74" spans="5:7" ht="15.75" thickBot="1">
+    <row r="74" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E74">
         <v>73</v>
       </c>
@@ -6310,7 +6321,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="75" spans="5:7" ht="15.75" thickBot="1">
+    <row r="75" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E75">
         <v>74</v>
       </c>
@@ -6321,7 +6332,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="76" spans="5:7" ht="15.75" thickBot="1">
+    <row r="76" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E76">
         <v>75</v>
       </c>
@@ -6332,7 +6343,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="77" spans="5:7" ht="15.75" thickBot="1">
+    <row r="77" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E77">
         <v>76</v>
       </c>
@@ -6343,7 +6354,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="78" spans="5:7" ht="15.75" thickBot="1">
+    <row r="78" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E78">
         <v>77</v>
       </c>
@@ -6354,7 +6365,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="79" spans="5:7" ht="15.75" thickBot="1">
+    <row r="79" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E79">
         <v>78</v>
       </c>
@@ -6365,7 +6376,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="80" spans="5:7" ht="15.75" thickBot="1">
+    <row r="80" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E80">
         <v>79</v>
       </c>
@@ -6376,7 +6387,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="81" spans="5:7" ht="15.75" thickBot="1">
+    <row r="81" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E81">
         <v>80</v>
       </c>
@@ -6387,7 +6398,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="82" spans="5:7" ht="15.75" thickBot="1">
+    <row r="82" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E82">
         <v>81</v>
       </c>
@@ -6398,7 +6409,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="83" spans="5:7" ht="15.75" thickBot="1">
+    <row r="83" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E83">
         <v>82</v>
       </c>
@@ -6409,7 +6420,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="84" spans="5:7" ht="15.75" thickBot="1">
+    <row r="84" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E84">
         <v>83</v>
       </c>
@@ -6420,7 +6431,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="85" spans="5:7" ht="15.75" thickBot="1">
+    <row r="85" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E85">
         <v>84</v>
       </c>
@@ -6431,201 +6442,201 @@
         <v>199</v>
       </c>
     </row>
-    <row r="86" spans="5:7" ht="15.75" thickBot="1">
+    <row r="86" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F86" s="17"/>
       <c r="G86" s="17"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" display="https://www.forbes.com/companies/ibm/?list=best-management-consulting-firms"/>
-    <hyperlink ref="G2" r:id="rId2" display="http://www.ibm.com/"/>
-    <hyperlink ref="F3" r:id="rId3" display="https://www.forbes.com/companies/dxc-technology/?list=best-management-consulting-firms"/>
-    <hyperlink ref="G3" r:id="rId4" display="http://www.dxc.technology/"/>
-    <hyperlink ref="F4" r:id="rId5" display="https://www.forbes.com/companies/deloitte-touche-tohmatsu/?list=best-management-consulting-firms"/>
-    <hyperlink ref="G4" r:id="rId6" display="http://www.deloitte.com/"/>
-    <hyperlink ref="F5" r:id="rId7" display="https://www.forbes.com/companies/cisco-systems/?list=best-management-consulting-firms"/>
-    <hyperlink ref="G5" r:id="rId8" display="http://www.cisco.com/"/>
-    <hyperlink ref="F6" r:id="rId9" display="https://www.forbes.com/companies/accenture/?list=best-management-consulting-firms"/>
-    <hyperlink ref="G6" r:id="rId10" display="http://www.accenture.com/"/>
-    <hyperlink ref="F7" r:id="rId11" display="https://www.forbes.com/companies/sap/?list=best-management-consulting-firms"/>
-    <hyperlink ref="G7" r:id="rId12" display="http://www.sap.com/"/>
-    <hyperlink ref="F8" r:id="rId13" display="https://www.forbes.com/companies/pricewaterhousecoopers/?list=best-management-consulting-firms"/>
-    <hyperlink ref="G8" r:id="rId14" display="http://www.pwc.com/"/>
-    <hyperlink ref="F9" r:id="rId15" display="https://www.forbes.com/companies/oracle/?list=best-management-consulting-firms"/>
-    <hyperlink ref="G9" r:id="rId16" display="http://www.oracle.com/"/>
-    <hyperlink ref="F10" r:id="rId17" display="https://www.forbes.com/companies/mckinsey-company/?list=best-management-consulting-firms"/>
-    <hyperlink ref="G10" r:id="rId18" display="http://www.mckinsey.com/"/>
-    <hyperlink ref="F11" r:id="rId19" display="https://www.forbes.com/companies/kpmg/?list=best-management-consulting-firms"/>
-    <hyperlink ref="G11" r:id="rId20" display="http://www.kpmg.com/"/>
-    <hyperlink ref="F12" r:id="rId21" display="https://www.forbes.com/companies/infosys-consulting/?list=best-management-consulting-firms"/>
-    <hyperlink ref="G12" r:id="rId22" display="http://www.infosys.com/"/>
-    <hyperlink ref="F13" r:id="rId23" display="https://www.forbes.com/companies/information-services-group/?list=best-management-consulting-firms"/>
-    <hyperlink ref="G13" r:id="rId24" display="http://www.isg-one.com/"/>
-    <hyperlink ref="F14" r:id="rId25" display="https://www.forbes.com/companies/gartner/?list=best-management-consulting-firms"/>
-    <hyperlink ref="G14" r:id="rId26" display="http://www.gartner.com/"/>
-    <hyperlink ref="F15" r:id="rId27" display="https://www.forbes.com/companies/ernst-young/?list=best-management-consulting-firms"/>
-    <hyperlink ref="G15" r:id="rId28" display="http://www.ey.com/"/>
-    <hyperlink ref="F16" r:id="rId29" display="https://www.forbes.com/companies/boston-consulting-group/?list=best-management-consulting-firms"/>
-    <hyperlink ref="G16" r:id="rId30" display="http://www.bcg.com/"/>
-    <hyperlink ref="F17" r:id="rId31" display="https://www.forbes.com/companies/booz-allen-hamilton/?list=best-management-consulting-firms"/>
-    <hyperlink ref="G17" r:id="rId32" display="http://www.boozallen.com/"/>
-    <hyperlink ref="F18" r:id="rId33" display="https://www.forbes.com/companies/west-monroe-partners/?list=best-management-consulting-firms"/>
-    <hyperlink ref="G18" r:id="rId34" display="http://www.westmonroepartners.com/"/>
-    <hyperlink ref="F19" r:id="rId35" display="https://www.forbes.com/companies/the-chartis-group/?list=best-management-consulting-firms"/>
-    <hyperlink ref="G19" r:id="rId36" display="http://www.chartis.com/"/>
-    <hyperlink ref="F20" r:id="rId37" display="https://www.forbes.com/companies/tata-consultancy-services/?list=best-management-consulting-firms"/>
-    <hyperlink ref="G20" r:id="rId38" display="http://www.tcs.com/"/>
-    <hyperlink ref="F21" r:id="rId39" display="https://www.forbes.com/companies/strategy/?list=best-management-consulting-firms"/>
-    <hyperlink ref="G21" r:id="rId40" display="http://www.strategyand.pwc.com/"/>
-    <hyperlink ref="F22" r:id="rId41" display="https://www.forbes.com/companies/ssa-company/?list=best-management-consulting-firms"/>
-    <hyperlink ref="G22" r:id="rId42" display="http://www.ssaandco.com/"/>
-    <hyperlink ref="F23" r:id="rId43" display="https://www.forbes.com/companies/slalom-consulting/?list=best-management-consulting-firms"/>
-    <hyperlink ref="G23" r:id="rId44" display="http://www.slalom.com/"/>
-    <hyperlink ref="F24" r:id="rId45" display="https://www.forbes.com/companies/sapient/?list=best-management-consulting-firms"/>
-    <hyperlink ref="G24" r:id="rId46" display="http://www.sapientconsulting.com/"/>
-    <hyperlink ref="F25" r:id="rId47" display="https://www.forbes.com/companies/roland-berger-strategy-consultants/?list=best-management-consulting-firms"/>
-    <hyperlink ref="G25" r:id="rId48" display="http://www.rolandberger.com/"/>
-    <hyperlink ref="F26" r:id="rId49" display="https://www.forbes.com/companies/resources-global-professionals/?list=best-management-consulting-firms"/>
-    <hyperlink ref="G26" r:id="rId50" display="http://www.rgp.com/"/>
-    <hyperlink ref="F27" r:id="rId51" display="https://www.forbes.com/companies/protiviti/?list=best-management-consulting-firms"/>
-    <hyperlink ref="G27" r:id="rId52" display="http://www.protiviti.com/"/>
-    <hyperlink ref="F28" r:id="rId53" display="https://www.forbes.com/companies/point-b/?list=best-management-consulting-firms"/>
-    <hyperlink ref="G28" r:id="rId54" display="http://www.pointb.com/"/>
-    <hyperlink ref="F29" r:id="rId55" display="https://www.forbes.com/companies/oliver-wyman/?list=best-management-consulting-firms"/>
-    <hyperlink ref="G29" r:id="rId56" display="http://www.oliverwyman.com/"/>
-    <hyperlink ref="F30" r:id="rId57" display="https://www.forbes.com/companies/oasys-international/?list=best-management-consulting-firms"/>
-    <hyperlink ref="G30" r:id="rId58" display="http://www.oasysic.com/"/>
-    <hyperlink ref="F31" r:id="rId59" display="https://www.forbes.com/companies/novantas/?list=best-management-consulting-firms"/>
-    <hyperlink ref="G31" r:id="rId60" display="http://www.novantas.com/"/>
-    <hyperlink ref="F32" r:id="rId61" display="https://www.forbes.com/companies/north-highland/?list=best-management-consulting-firms"/>
-    <hyperlink ref="G32" r:id="rId62" display="http://www.northhighland.com/"/>
-    <hyperlink ref="F33" r:id="rId63" display="https://www.forbes.com/companies/medmatica-consulting-associates/?list=best-management-consulting-firms"/>
-    <hyperlink ref="G33" r:id="rId64" display="http://www.medmatica.com/"/>
-    <hyperlink ref="F34" r:id="rId65" display="https://www.forbes.com/companies/lockheed-martin/?list=best-management-consulting-firms"/>
-    <hyperlink ref="G34" r:id="rId66" display="http://www.lockheedmartin.com/"/>
-    <hyperlink ref="F35" r:id="rId67" display="https://www.forbes.com/companies/leappoint/?list=best-management-consulting-firms"/>
-    <hyperlink ref="G35" r:id="rId68" display="http://leappoint.com/"/>
-    <hyperlink ref="F36" r:id="rId69" display="https://www.forbes.com/companies/kurt-salmon/?list=best-management-consulting-firms"/>
-    <hyperlink ref="G36" r:id="rId70" display="http://www.kurtsalmon.com/"/>
-    <hyperlink ref="F37" r:id="rId71" display="https://www.forbes.com/companies/jabian-consulting/?list=best-management-consulting-firms"/>
-    <hyperlink ref="G37" r:id="rId72" display="http://www.jabian.com/"/>
-    <hyperlink ref="F38" r:id="rId73" display="https://www.forbes.com/companies/impact-advisors/?list=best-management-consulting-firms"/>
-    <hyperlink ref="G38" r:id="rId74" display="http://www.impact-advisors.com/"/>
-    <hyperlink ref="F39" r:id="rId75" display="https://www.forbes.com/companies/ignyte-group/?list=best-management-consulting-firms"/>
-    <hyperlink ref="G39" r:id="rId76" display="http://ignytegroup.com/"/>
-    <hyperlink ref="F40" r:id="rId77" display="https://www.forbes.com/companies/huron-consulting-group/?list=best-management-consulting-firms"/>
-    <hyperlink ref="G40" r:id="rId78" display="http://www.huronconsultinggroup.com/"/>
-    <hyperlink ref="F41" r:id="rId79" display="https://www.forbes.com/companies/grant-thornton/?list=best-management-consulting-firms"/>
-    <hyperlink ref="G41" r:id="rId80" display="http://www.grantthornton.com/"/>
-    <hyperlink ref="F42" r:id="rId81" display="https://www.forbes.com/companies/fti-consulting/?list=best-management-consulting-firms"/>
-    <hyperlink ref="G42" r:id="rId82" display="http://www.fticonsulting.com/"/>
-    <hyperlink ref="F43" r:id="rId83" display="https://www.forbes.com/companies/forsythe-solutions-group/?list=best-management-consulting-firms"/>
-    <hyperlink ref="G43" r:id="rId84" display="http://www.forsythe.com/"/>
-    <hyperlink ref="F44" r:id="rId85" display="https://www.forbes.com/companies/everest-group/?list=best-management-consulting-firms"/>
-    <hyperlink ref="G44" r:id="rId86" display="http://www.everestgrp.com/"/>
-    <hyperlink ref="F45" r:id="rId87" display="https://www.forbes.com/companies/cumberland-consulting-group/?list=best-management-consulting-firms"/>
-    <hyperlink ref="G45" r:id="rId88" display="http://www.cumberlandcg.com/"/>
-    <hyperlink ref="F46" r:id="rId89" display="https://www.forbes.com/companies/cognizant/?list=best-management-consulting-firms"/>
-    <hyperlink ref="G46" r:id="rId90" display="http://www.cognizant.com/"/>
-    <hyperlink ref="F47" r:id="rId91" display="https://www.forbes.com/companies/clarkston-consulting/?list=best-management-consulting-firms"/>
-    <hyperlink ref="G47" r:id="rId92" display="http://www.clarkstonconsulting.com/"/>
-    <hyperlink ref="F48" r:id="rId93" display="https://www.forbes.com/companies/cgn-global/?list=best-management-consulting-firms"/>
-    <hyperlink ref="G48" r:id="rId94" display="http://www.cgnglobal.com/"/>
-    <hyperlink ref="F49" r:id="rId95" display="https://www.forbes.com/companies/censeo-consulting-group/?list=best-management-consulting-firms"/>
-    <hyperlink ref="G49" r:id="rId96" display="http://www.censeoconsulting.com/"/>
-    <hyperlink ref="F50" r:id="rId97" display="https://www.forbes.com/companies/captech/?list=best-management-consulting-firms"/>
-    <hyperlink ref="G50" r:id="rId98" display="http://www.captechconsulting.com/"/>
-    <hyperlink ref="F51" r:id="rId99" display="https://www.forbes.com/companies/capgemini-consulting/?list=best-management-consulting-firms"/>
-    <hyperlink ref="G51" r:id="rId100" display="http://www.capgemini.com/"/>
-    <hyperlink ref="F52" r:id="rId101" display="https://www.forbes.com/companies/brattle-group/?list=best-management-consulting-firms"/>
-    <hyperlink ref="G52" r:id="rId102" display="http://www.brattle.com/"/>
-    <hyperlink ref="F53" r:id="rId103" display="https://www.forbes.com/companies/bdo-usa/?list=best-management-consulting-firms"/>
-    <hyperlink ref="G53" r:id="rId104" display="http://www.bdo.com/"/>
-    <hyperlink ref="F54" r:id="rId105" display="https://www.forbes.com/companies/bain-and-company/?list=best-management-consulting-firms"/>
-    <hyperlink ref="G54" r:id="rId106" display="http://www.bain.com/"/>
-    <hyperlink ref="F55" r:id="rId107" display="https://www.forbes.com/companies/bae-systems/?list=best-management-consulting-firms"/>
-    <hyperlink ref="G55" r:id="rId108" display="http://www.baesystems.com/"/>
-    <hyperlink ref="F56" r:id="rId109" display="https://www.forbes.com/companies/avasant/?list=best-management-consulting-firms"/>
-    <hyperlink ref="G56" r:id="rId110" display="http://www.avasant.com/"/>
-    <hyperlink ref="F57" r:id="rId111" display="https://www.forbes.com/companies/at-kearney/?list=best-management-consulting-firms"/>
-    <hyperlink ref="G57" r:id="rId112" display="http://www.atkearney.com/"/>
-    <hyperlink ref="F58" r:id="rId113" display="https://www.forbes.com/companies/arthur-d-little/?list=best-management-consulting-firms"/>
-    <hyperlink ref="G58" r:id="rId114" display="http://www.adlittle.com/"/>
-    <hyperlink ref="F59" r:id="rId115" display="https://www.forbes.com/companies/archpoint/?list=best-management-consulting-firms"/>
-    <hyperlink ref="G59" r:id="rId116" display="http://www.archpointconsulting.com/"/>
-    <hyperlink ref="F60" r:id="rId117" display="https://www.forbes.com/companies/appirio/?list=best-management-consulting-firms"/>
-    <hyperlink ref="G60" r:id="rId118" display="http://www.appirio.com/"/>
-    <hyperlink ref="F61" r:id="rId119" display="https://www.forbes.com/companies/alixpartners/?list=best-management-consulting-firms"/>
-    <hyperlink ref="G61" r:id="rId120" display="http://www.alixpartners.com/"/>
-    <hyperlink ref="F62" r:id="rId121" display="https://www.forbes.com/companies/microsoft/?list=best-management-consulting-firms"/>
-    <hyperlink ref="G62" r:id="rId122" display="http://www.microsoft.com/"/>
-    <hyperlink ref="F63" r:id="rId123" display="https://www.forbes.com/companies/wipro/?list=best-management-consulting-firms"/>
-    <hyperlink ref="G63" r:id="rId124" display="http://www.wipro.com/"/>
-    <hyperlink ref="F64" r:id="rId125" display="https://www.forbes.com/companies/virtusa/?list=best-management-consulting-firms"/>
-    <hyperlink ref="G64" r:id="rId126" display="http://www.virtusa.com/"/>
-    <hyperlink ref="F65" r:id="rId127" display="https://www.forbes.com/companies/ntt-data-services/?list=best-management-consulting-firms"/>
-    <hyperlink ref="G65" r:id="rId128" display="http://us.nttdata.com/"/>
-    <hyperlink ref="F66" r:id="rId129" display="https://www.forbes.com/companies/mckinnis-consulting-services/?list=best-management-consulting-firms"/>
-    <hyperlink ref="G66" r:id="rId130" display="http://www.mckinnisconsulting.com/"/>
-    <hyperlink ref="F67" r:id="rId131" display="https://www.forbes.com/companies/hitachi-consulting/?list=best-management-consulting-firms"/>
-    <hyperlink ref="G67" r:id="rId132" display="http://www.hitachiconsulting.com/"/>
-    <hyperlink ref="F68" r:id="rId133" display="https://www.forbes.com/companies/hcl-technologies/?list=best-management-consulting-firms"/>
-    <hyperlink ref="G68" r:id="rId134" display="http://www.hcltech.com/"/>
-    <hyperlink ref="F69" r:id="rId135" display="https://www.forbes.com/companies/fujitsu-america/?list=best-management-consulting-firms"/>
-    <hyperlink ref="G69" r:id="rId136" display="http://www.fujitsu.com/"/>
-    <hyperlink ref="F70" r:id="rId137" display="https://www.forbes.com/companies/bridge-solutions-group/?list=best-management-consulting-firms"/>
-    <hyperlink ref="G70" r:id="rId138" display="http://bridgesgi.com/"/>
-    <hyperlink ref="F71" r:id="rId139" display="https://www.forbes.com/companies/blue-horseshoe-solutions/?list=best-management-consulting-firms"/>
-    <hyperlink ref="G71" r:id="rId140" display="http://www.bhsolutions.com/"/>
-    <hyperlink ref="F72" r:id="rId141" display="https://www.forbes.com/companies/application-consulting-group/?list=best-management-consulting-firms"/>
-    <hyperlink ref="G72" r:id="rId142" display="http://www.acgi.com/"/>
-    <hyperlink ref="F73" r:id="rId143" display="https://www.forbes.com/companies/simon-kucher-partners/?list=best-management-consulting-firms"/>
-    <hyperlink ref="G73" r:id="rId144" display="http://www.simon-kucher.com/"/>
-    <hyperlink ref="F74" r:id="rId145" display="https://www.forbes.com/companies/navigant-consulting/?list=best-management-consulting-firms"/>
-    <hyperlink ref="G74" r:id="rId146" display="http://www.navigant.com/"/>
-    <hyperlink ref="F75" r:id="rId147" display="https://www.forbes.com/companies/keystone-strategy/?list=best-management-consulting-firms"/>
-    <hyperlink ref="G75" r:id="rId148" display="http://www.keystonestrategy.com/"/>
-    <hyperlink ref="F76" r:id="rId149" display="https://www.forbes.com/companies/kaiser-associates/?list=best-management-consulting-firms"/>
-    <hyperlink ref="G76" r:id="rId150" display="http://www.kaiserassociates.com/"/>
-    <hyperlink ref="F77" r:id="rId151" display="https://www.forbes.com/companies/insight-sourcing-group/?list=best-management-consulting-firms"/>
-    <hyperlink ref="G77" r:id="rId152" display="http://www.insightsourcing.com/"/>
-    <hyperlink ref="F78" r:id="rId153" display="https://www.forbes.com/companies/innosight/?list=best-management-consulting-firms"/>
-    <hyperlink ref="G78" r:id="rId154" display="http://www.innosight.com/"/>
-    <hyperlink ref="F79" r:id="rId155" display="https://www.forbes.com/companies/ibb-consulting-group/?list=best-management-consulting-firms"/>
-    <hyperlink ref="G79" r:id="rId156" display="http://www.ibbconsulting.com/"/>
-    <hyperlink ref="F80" r:id="rId157" display="https://www.forbes.com/companies/hay-group/?list=best-management-consulting-firms"/>
-    <hyperlink ref="G80" r:id="rId158" display="http://www.haygroup.com/"/>
-    <hyperlink ref="F81" r:id="rId159" display="https://www.forbes.com/companies/cornerstone-research/?list=best-management-consulting-firms"/>
-    <hyperlink ref="G81" r:id="rId160" display="http://www.cornerstone.com/"/>
-    <hyperlink ref="F82" r:id="rId161" display="https://www.forbes.com/companies/charles-river-associates/?list=best-management-consulting-firms"/>
-    <hyperlink ref="G82" r:id="rId162" display="http://www.crai.com/"/>
-    <hyperlink ref="F83" r:id="rId163" display="https://www.forbes.com/companies/centric-consulting/?list=best-management-consulting-firms"/>
-    <hyperlink ref="G83" r:id="rId164" display="http://www.centricconsulting.com/"/>
-    <hyperlink ref="F84" r:id="rId165" display="https://www.forbes.com/companies/bates-white/?list=best-management-consulting-firms"/>
-    <hyperlink ref="G84" r:id="rId166" display="http://www.bateswhite.com/"/>
-    <hyperlink ref="F85" r:id="rId167" display="https://www.forbes.com/companies/avanade/?list=best-management-consulting-firms"/>
-    <hyperlink ref="G85" r:id="rId168" display="http://www.avanade.com/"/>
+    <hyperlink ref="F2" r:id="rId1" display="https://www.forbes.com/companies/ibm/?list=best-management-consulting-firms" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="G2" r:id="rId2" display="http://www.ibm.com/" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="F3" r:id="rId3" display="https://www.forbes.com/companies/dxc-technology/?list=best-management-consulting-firms" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="G3" r:id="rId4" display="http://www.dxc.technology/" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="F4" r:id="rId5" display="https://www.forbes.com/companies/deloitte-touche-tohmatsu/?list=best-management-consulting-firms" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
+    <hyperlink ref="G4" r:id="rId6" display="http://www.deloitte.com/" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
+    <hyperlink ref="F5" r:id="rId7" display="https://www.forbes.com/companies/cisco-systems/?list=best-management-consulting-firms" xr:uid="{00000000-0004-0000-0200-000006000000}"/>
+    <hyperlink ref="G5" r:id="rId8" display="http://www.cisco.com/" xr:uid="{00000000-0004-0000-0200-000007000000}"/>
+    <hyperlink ref="F6" r:id="rId9" display="https://www.forbes.com/companies/accenture/?list=best-management-consulting-firms" xr:uid="{00000000-0004-0000-0200-000008000000}"/>
+    <hyperlink ref="G6" r:id="rId10" display="http://www.accenture.com/" xr:uid="{00000000-0004-0000-0200-000009000000}"/>
+    <hyperlink ref="F7" r:id="rId11" display="https://www.forbes.com/companies/sap/?list=best-management-consulting-firms" xr:uid="{00000000-0004-0000-0200-00000A000000}"/>
+    <hyperlink ref="G7" r:id="rId12" display="http://www.sap.com/" xr:uid="{00000000-0004-0000-0200-00000B000000}"/>
+    <hyperlink ref="F8" r:id="rId13" display="https://www.forbes.com/companies/pricewaterhousecoopers/?list=best-management-consulting-firms" xr:uid="{00000000-0004-0000-0200-00000C000000}"/>
+    <hyperlink ref="G8" r:id="rId14" display="http://www.pwc.com/" xr:uid="{00000000-0004-0000-0200-00000D000000}"/>
+    <hyperlink ref="F9" r:id="rId15" display="https://www.forbes.com/companies/oracle/?list=best-management-consulting-firms" xr:uid="{00000000-0004-0000-0200-00000E000000}"/>
+    <hyperlink ref="G9" r:id="rId16" display="http://www.oracle.com/" xr:uid="{00000000-0004-0000-0200-00000F000000}"/>
+    <hyperlink ref="F10" r:id="rId17" display="https://www.forbes.com/companies/mckinsey-company/?list=best-management-consulting-firms" xr:uid="{00000000-0004-0000-0200-000010000000}"/>
+    <hyperlink ref="G10" r:id="rId18" display="http://www.mckinsey.com/" xr:uid="{00000000-0004-0000-0200-000011000000}"/>
+    <hyperlink ref="F11" r:id="rId19" display="https://www.forbes.com/companies/kpmg/?list=best-management-consulting-firms" xr:uid="{00000000-0004-0000-0200-000012000000}"/>
+    <hyperlink ref="G11" r:id="rId20" display="http://www.kpmg.com/" xr:uid="{00000000-0004-0000-0200-000013000000}"/>
+    <hyperlink ref="F12" r:id="rId21" display="https://www.forbes.com/companies/infosys-consulting/?list=best-management-consulting-firms" xr:uid="{00000000-0004-0000-0200-000014000000}"/>
+    <hyperlink ref="G12" r:id="rId22" display="http://www.infosys.com/" xr:uid="{00000000-0004-0000-0200-000015000000}"/>
+    <hyperlink ref="F13" r:id="rId23" display="https://www.forbes.com/companies/information-services-group/?list=best-management-consulting-firms" xr:uid="{00000000-0004-0000-0200-000016000000}"/>
+    <hyperlink ref="G13" r:id="rId24" display="http://www.isg-one.com/" xr:uid="{00000000-0004-0000-0200-000017000000}"/>
+    <hyperlink ref="F14" r:id="rId25" display="https://www.forbes.com/companies/gartner/?list=best-management-consulting-firms" xr:uid="{00000000-0004-0000-0200-000018000000}"/>
+    <hyperlink ref="G14" r:id="rId26" display="http://www.gartner.com/" xr:uid="{00000000-0004-0000-0200-000019000000}"/>
+    <hyperlink ref="F15" r:id="rId27" display="https://www.forbes.com/companies/ernst-young/?list=best-management-consulting-firms" xr:uid="{00000000-0004-0000-0200-00001A000000}"/>
+    <hyperlink ref="G15" r:id="rId28" display="http://www.ey.com/" xr:uid="{00000000-0004-0000-0200-00001B000000}"/>
+    <hyperlink ref="F16" r:id="rId29" display="https://www.forbes.com/companies/boston-consulting-group/?list=best-management-consulting-firms" xr:uid="{00000000-0004-0000-0200-00001C000000}"/>
+    <hyperlink ref="G16" r:id="rId30" display="http://www.bcg.com/" xr:uid="{00000000-0004-0000-0200-00001D000000}"/>
+    <hyperlink ref="F17" r:id="rId31" display="https://www.forbes.com/companies/booz-allen-hamilton/?list=best-management-consulting-firms" xr:uid="{00000000-0004-0000-0200-00001E000000}"/>
+    <hyperlink ref="G17" r:id="rId32" display="http://www.boozallen.com/" xr:uid="{00000000-0004-0000-0200-00001F000000}"/>
+    <hyperlink ref="F18" r:id="rId33" display="https://www.forbes.com/companies/west-monroe-partners/?list=best-management-consulting-firms" xr:uid="{00000000-0004-0000-0200-000020000000}"/>
+    <hyperlink ref="G18" r:id="rId34" display="http://www.westmonroepartners.com/" xr:uid="{00000000-0004-0000-0200-000021000000}"/>
+    <hyperlink ref="F19" r:id="rId35" display="https://www.forbes.com/companies/the-chartis-group/?list=best-management-consulting-firms" xr:uid="{00000000-0004-0000-0200-000022000000}"/>
+    <hyperlink ref="G19" r:id="rId36" display="http://www.chartis.com/" xr:uid="{00000000-0004-0000-0200-000023000000}"/>
+    <hyperlink ref="F20" r:id="rId37" display="https://www.forbes.com/companies/tata-consultancy-services/?list=best-management-consulting-firms" xr:uid="{00000000-0004-0000-0200-000024000000}"/>
+    <hyperlink ref="G20" r:id="rId38" display="http://www.tcs.com/" xr:uid="{00000000-0004-0000-0200-000025000000}"/>
+    <hyperlink ref="F21" r:id="rId39" display="https://www.forbes.com/companies/strategy/?list=best-management-consulting-firms" xr:uid="{00000000-0004-0000-0200-000026000000}"/>
+    <hyperlink ref="G21" r:id="rId40" display="http://www.strategyand.pwc.com/" xr:uid="{00000000-0004-0000-0200-000027000000}"/>
+    <hyperlink ref="F22" r:id="rId41" display="https://www.forbes.com/companies/ssa-company/?list=best-management-consulting-firms" xr:uid="{00000000-0004-0000-0200-000028000000}"/>
+    <hyperlink ref="G22" r:id="rId42" display="http://www.ssaandco.com/" xr:uid="{00000000-0004-0000-0200-000029000000}"/>
+    <hyperlink ref="F23" r:id="rId43" display="https://www.forbes.com/companies/slalom-consulting/?list=best-management-consulting-firms" xr:uid="{00000000-0004-0000-0200-00002A000000}"/>
+    <hyperlink ref="G23" r:id="rId44" display="http://www.slalom.com/" xr:uid="{00000000-0004-0000-0200-00002B000000}"/>
+    <hyperlink ref="F24" r:id="rId45" display="https://www.forbes.com/companies/sapient/?list=best-management-consulting-firms" xr:uid="{00000000-0004-0000-0200-00002C000000}"/>
+    <hyperlink ref="G24" r:id="rId46" display="http://www.sapientconsulting.com/" xr:uid="{00000000-0004-0000-0200-00002D000000}"/>
+    <hyperlink ref="F25" r:id="rId47" display="https://www.forbes.com/companies/roland-berger-strategy-consultants/?list=best-management-consulting-firms" xr:uid="{00000000-0004-0000-0200-00002E000000}"/>
+    <hyperlink ref="G25" r:id="rId48" display="http://www.rolandberger.com/" xr:uid="{00000000-0004-0000-0200-00002F000000}"/>
+    <hyperlink ref="F26" r:id="rId49" display="https://www.forbes.com/companies/resources-global-professionals/?list=best-management-consulting-firms" xr:uid="{00000000-0004-0000-0200-000030000000}"/>
+    <hyperlink ref="G26" r:id="rId50" display="http://www.rgp.com/" xr:uid="{00000000-0004-0000-0200-000031000000}"/>
+    <hyperlink ref="F27" r:id="rId51" display="https://www.forbes.com/companies/protiviti/?list=best-management-consulting-firms" xr:uid="{00000000-0004-0000-0200-000032000000}"/>
+    <hyperlink ref="G27" r:id="rId52" display="http://www.protiviti.com/" xr:uid="{00000000-0004-0000-0200-000033000000}"/>
+    <hyperlink ref="F28" r:id="rId53" display="https://www.forbes.com/companies/point-b/?list=best-management-consulting-firms" xr:uid="{00000000-0004-0000-0200-000034000000}"/>
+    <hyperlink ref="G28" r:id="rId54" display="http://www.pointb.com/" xr:uid="{00000000-0004-0000-0200-000035000000}"/>
+    <hyperlink ref="F29" r:id="rId55" display="https://www.forbes.com/companies/oliver-wyman/?list=best-management-consulting-firms" xr:uid="{00000000-0004-0000-0200-000036000000}"/>
+    <hyperlink ref="G29" r:id="rId56" display="http://www.oliverwyman.com/" xr:uid="{00000000-0004-0000-0200-000037000000}"/>
+    <hyperlink ref="F30" r:id="rId57" display="https://www.forbes.com/companies/oasys-international/?list=best-management-consulting-firms" xr:uid="{00000000-0004-0000-0200-000038000000}"/>
+    <hyperlink ref="G30" r:id="rId58" display="http://www.oasysic.com/" xr:uid="{00000000-0004-0000-0200-000039000000}"/>
+    <hyperlink ref="F31" r:id="rId59" display="https://www.forbes.com/companies/novantas/?list=best-management-consulting-firms" xr:uid="{00000000-0004-0000-0200-00003A000000}"/>
+    <hyperlink ref="G31" r:id="rId60" display="http://www.novantas.com/" xr:uid="{00000000-0004-0000-0200-00003B000000}"/>
+    <hyperlink ref="F32" r:id="rId61" display="https://www.forbes.com/companies/north-highland/?list=best-management-consulting-firms" xr:uid="{00000000-0004-0000-0200-00003C000000}"/>
+    <hyperlink ref="G32" r:id="rId62" display="http://www.northhighland.com/" xr:uid="{00000000-0004-0000-0200-00003D000000}"/>
+    <hyperlink ref="F33" r:id="rId63" display="https://www.forbes.com/companies/medmatica-consulting-associates/?list=best-management-consulting-firms" xr:uid="{00000000-0004-0000-0200-00003E000000}"/>
+    <hyperlink ref="G33" r:id="rId64" display="http://www.medmatica.com/" xr:uid="{00000000-0004-0000-0200-00003F000000}"/>
+    <hyperlink ref="F34" r:id="rId65" display="https://www.forbes.com/companies/lockheed-martin/?list=best-management-consulting-firms" xr:uid="{00000000-0004-0000-0200-000040000000}"/>
+    <hyperlink ref="G34" r:id="rId66" display="http://www.lockheedmartin.com/" xr:uid="{00000000-0004-0000-0200-000041000000}"/>
+    <hyperlink ref="F35" r:id="rId67" display="https://www.forbes.com/companies/leappoint/?list=best-management-consulting-firms" xr:uid="{00000000-0004-0000-0200-000042000000}"/>
+    <hyperlink ref="G35" r:id="rId68" display="http://leappoint.com/" xr:uid="{00000000-0004-0000-0200-000043000000}"/>
+    <hyperlink ref="F36" r:id="rId69" display="https://www.forbes.com/companies/kurt-salmon/?list=best-management-consulting-firms" xr:uid="{00000000-0004-0000-0200-000044000000}"/>
+    <hyperlink ref="G36" r:id="rId70" display="http://www.kurtsalmon.com/" xr:uid="{00000000-0004-0000-0200-000045000000}"/>
+    <hyperlink ref="F37" r:id="rId71" display="https://www.forbes.com/companies/jabian-consulting/?list=best-management-consulting-firms" xr:uid="{00000000-0004-0000-0200-000046000000}"/>
+    <hyperlink ref="G37" r:id="rId72" display="http://www.jabian.com/" xr:uid="{00000000-0004-0000-0200-000047000000}"/>
+    <hyperlink ref="F38" r:id="rId73" display="https://www.forbes.com/companies/impact-advisors/?list=best-management-consulting-firms" xr:uid="{00000000-0004-0000-0200-000048000000}"/>
+    <hyperlink ref="G38" r:id="rId74" display="http://www.impact-advisors.com/" xr:uid="{00000000-0004-0000-0200-000049000000}"/>
+    <hyperlink ref="F39" r:id="rId75" display="https://www.forbes.com/companies/ignyte-group/?list=best-management-consulting-firms" xr:uid="{00000000-0004-0000-0200-00004A000000}"/>
+    <hyperlink ref="G39" r:id="rId76" display="http://ignytegroup.com/" xr:uid="{00000000-0004-0000-0200-00004B000000}"/>
+    <hyperlink ref="F40" r:id="rId77" display="https://www.forbes.com/companies/huron-consulting-group/?list=best-management-consulting-firms" xr:uid="{00000000-0004-0000-0200-00004C000000}"/>
+    <hyperlink ref="G40" r:id="rId78" display="http://www.huronconsultinggroup.com/" xr:uid="{00000000-0004-0000-0200-00004D000000}"/>
+    <hyperlink ref="F41" r:id="rId79" display="https://www.forbes.com/companies/grant-thornton/?list=best-management-consulting-firms" xr:uid="{00000000-0004-0000-0200-00004E000000}"/>
+    <hyperlink ref="G41" r:id="rId80" display="http://www.grantthornton.com/" xr:uid="{00000000-0004-0000-0200-00004F000000}"/>
+    <hyperlink ref="F42" r:id="rId81" display="https://www.forbes.com/companies/fti-consulting/?list=best-management-consulting-firms" xr:uid="{00000000-0004-0000-0200-000050000000}"/>
+    <hyperlink ref="G42" r:id="rId82" display="http://www.fticonsulting.com/" xr:uid="{00000000-0004-0000-0200-000051000000}"/>
+    <hyperlink ref="F43" r:id="rId83" display="https://www.forbes.com/companies/forsythe-solutions-group/?list=best-management-consulting-firms" xr:uid="{00000000-0004-0000-0200-000052000000}"/>
+    <hyperlink ref="G43" r:id="rId84" display="http://www.forsythe.com/" xr:uid="{00000000-0004-0000-0200-000053000000}"/>
+    <hyperlink ref="F44" r:id="rId85" display="https://www.forbes.com/companies/everest-group/?list=best-management-consulting-firms" xr:uid="{00000000-0004-0000-0200-000054000000}"/>
+    <hyperlink ref="G44" r:id="rId86" display="http://www.everestgrp.com/" xr:uid="{00000000-0004-0000-0200-000055000000}"/>
+    <hyperlink ref="F45" r:id="rId87" display="https://www.forbes.com/companies/cumberland-consulting-group/?list=best-management-consulting-firms" xr:uid="{00000000-0004-0000-0200-000056000000}"/>
+    <hyperlink ref="G45" r:id="rId88" display="http://www.cumberlandcg.com/" xr:uid="{00000000-0004-0000-0200-000057000000}"/>
+    <hyperlink ref="F46" r:id="rId89" display="https://www.forbes.com/companies/cognizant/?list=best-management-consulting-firms" xr:uid="{00000000-0004-0000-0200-000058000000}"/>
+    <hyperlink ref="G46" r:id="rId90" display="http://www.cognizant.com/" xr:uid="{00000000-0004-0000-0200-000059000000}"/>
+    <hyperlink ref="F47" r:id="rId91" display="https://www.forbes.com/companies/clarkston-consulting/?list=best-management-consulting-firms" xr:uid="{00000000-0004-0000-0200-00005A000000}"/>
+    <hyperlink ref="G47" r:id="rId92" display="http://www.clarkstonconsulting.com/" xr:uid="{00000000-0004-0000-0200-00005B000000}"/>
+    <hyperlink ref="F48" r:id="rId93" display="https://www.forbes.com/companies/cgn-global/?list=best-management-consulting-firms" xr:uid="{00000000-0004-0000-0200-00005C000000}"/>
+    <hyperlink ref="G48" r:id="rId94" display="http://www.cgnglobal.com/" xr:uid="{00000000-0004-0000-0200-00005D000000}"/>
+    <hyperlink ref="F49" r:id="rId95" display="https://www.forbes.com/companies/censeo-consulting-group/?list=best-management-consulting-firms" xr:uid="{00000000-0004-0000-0200-00005E000000}"/>
+    <hyperlink ref="G49" r:id="rId96" display="http://www.censeoconsulting.com/" xr:uid="{00000000-0004-0000-0200-00005F000000}"/>
+    <hyperlink ref="F50" r:id="rId97" display="https://www.forbes.com/companies/captech/?list=best-management-consulting-firms" xr:uid="{00000000-0004-0000-0200-000060000000}"/>
+    <hyperlink ref="G50" r:id="rId98" display="http://www.captechconsulting.com/" xr:uid="{00000000-0004-0000-0200-000061000000}"/>
+    <hyperlink ref="F51" r:id="rId99" display="https://www.forbes.com/companies/capgemini-consulting/?list=best-management-consulting-firms" xr:uid="{00000000-0004-0000-0200-000062000000}"/>
+    <hyperlink ref="G51" r:id="rId100" display="http://www.capgemini.com/" xr:uid="{00000000-0004-0000-0200-000063000000}"/>
+    <hyperlink ref="F52" r:id="rId101" display="https://www.forbes.com/companies/brattle-group/?list=best-management-consulting-firms" xr:uid="{00000000-0004-0000-0200-000064000000}"/>
+    <hyperlink ref="G52" r:id="rId102" display="http://www.brattle.com/" xr:uid="{00000000-0004-0000-0200-000065000000}"/>
+    <hyperlink ref="F53" r:id="rId103" display="https://www.forbes.com/companies/bdo-usa/?list=best-management-consulting-firms" xr:uid="{00000000-0004-0000-0200-000066000000}"/>
+    <hyperlink ref="G53" r:id="rId104" display="http://www.bdo.com/" xr:uid="{00000000-0004-0000-0200-000067000000}"/>
+    <hyperlink ref="F54" r:id="rId105" display="https://www.forbes.com/companies/bain-and-company/?list=best-management-consulting-firms" xr:uid="{00000000-0004-0000-0200-000068000000}"/>
+    <hyperlink ref="G54" r:id="rId106" display="http://www.bain.com/" xr:uid="{00000000-0004-0000-0200-000069000000}"/>
+    <hyperlink ref="F55" r:id="rId107" display="https://www.forbes.com/companies/bae-systems/?list=best-management-consulting-firms" xr:uid="{00000000-0004-0000-0200-00006A000000}"/>
+    <hyperlink ref="G55" r:id="rId108" display="http://www.baesystems.com/" xr:uid="{00000000-0004-0000-0200-00006B000000}"/>
+    <hyperlink ref="F56" r:id="rId109" display="https://www.forbes.com/companies/avasant/?list=best-management-consulting-firms" xr:uid="{00000000-0004-0000-0200-00006C000000}"/>
+    <hyperlink ref="G56" r:id="rId110" display="http://www.avasant.com/" xr:uid="{00000000-0004-0000-0200-00006D000000}"/>
+    <hyperlink ref="F57" r:id="rId111" display="https://www.forbes.com/companies/at-kearney/?list=best-management-consulting-firms" xr:uid="{00000000-0004-0000-0200-00006E000000}"/>
+    <hyperlink ref="G57" r:id="rId112" display="http://www.atkearney.com/" xr:uid="{00000000-0004-0000-0200-00006F000000}"/>
+    <hyperlink ref="F58" r:id="rId113" display="https://www.forbes.com/companies/arthur-d-little/?list=best-management-consulting-firms" xr:uid="{00000000-0004-0000-0200-000070000000}"/>
+    <hyperlink ref="G58" r:id="rId114" display="http://www.adlittle.com/" xr:uid="{00000000-0004-0000-0200-000071000000}"/>
+    <hyperlink ref="F59" r:id="rId115" display="https://www.forbes.com/companies/archpoint/?list=best-management-consulting-firms" xr:uid="{00000000-0004-0000-0200-000072000000}"/>
+    <hyperlink ref="G59" r:id="rId116" display="http://www.archpointconsulting.com/" xr:uid="{00000000-0004-0000-0200-000073000000}"/>
+    <hyperlink ref="F60" r:id="rId117" display="https://www.forbes.com/companies/appirio/?list=best-management-consulting-firms" xr:uid="{00000000-0004-0000-0200-000074000000}"/>
+    <hyperlink ref="G60" r:id="rId118" display="http://www.appirio.com/" xr:uid="{00000000-0004-0000-0200-000075000000}"/>
+    <hyperlink ref="F61" r:id="rId119" display="https://www.forbes.com/companies/alixpartners/?list=best-management-consulting-firms" xr:uid="{00000000-0004-0000-0200-000076000000}"/>
+    <hyperlink ref="G61" r:id="rId120" display="http://www.alixpartners.com/" xr:uid="{00000000-0004-0000-0200-000077000000}"/>
+    <hyperlink ref="F62" r:id="rId121" display="https://www.forbes.com/companies/microsoft/?list=best-management-consulting-firms" xr:uid="{00000000-0004-0000-0200-000078000000}"/>
+    <hyperlink ref="G62" r:id="rId122" display="http://www.microsoft.com/" xr:uid="{00000000-0004-0000-0200-000079000000}"/>
+    <hyperlink ref="F63" r:id="rId123" display="https://www.forbes.com/companies/wipro/?list=best-management-consulting-firms" xr:uid="{00000000-0004-0000-0200-00007A000000}"/>
+    <hyperlink ref="G63" r:id="rId124" display="http://www.wipro.com/" xr:uid="{00000000-0004-0000-0200-00007B000000}"/>
+    <hyperlink ref="F64" r:id="rId125" display="https://www.forbes.com/companies/virtusa/?list=best-management-consulting-firms" xr:uid="{00000000-0004-0000-0200-00007C000000}"/>
+    <hyperlink ref="G64" r:id="rId126" display="http://www.virtusa.com/" xr:uid="{00000000-0004-0000-0200-00007D000000}"/>
+    <hyperlink ref="F65" r:id="rId127" display="https://www.forbes.com/companies/ntt-data-services/?list=best-management-consulting-firms" xr:uid="{00000000-0004-0000-0200-00007E000000}"/>
+    <hyperlink ref="G65" r:id="rId128" display="http://us.nttdata.com/" xr:uid="{00000000-0004-0000-0200-00007F000000}"/>
+    <hyperlink ref="F66" r:id="rId129" display="https://www.forbes.com/companies/mckinnis-consulting-services/?list=best-management-consulting-firms" xr:uid="{00000000-0004-0000-0200-000080000000}"/>
+    <hyperlink ref="G66" r:id="rId130" display="http://www.mckinnisconsulting.com/" xr:uid="{00000000-0004-0000-0200-000081000000}"/>
+    <hyperlink ref="F67" r:id="rId131" display="https://www.forbes.com/companies/hitachi-consulting/?list=best-management-consulting-firms" xr:uid="{00000000-0004-0000-0200-000082000000}"/>
+    <hyperlink ref="G67" r:id="rId132" display="http://www.hitachiconsulting.com/" xr:uid="{00000000-0004-0000-0200-000083000000}"/>
+    <hyperlink ref="F68" r:id="rId133" display="https://www.forbes.com/companies/hcl-technologies/?list=best-management-consulting-firms" xr:uid="{00000000-0004-0000-0200-000084000000}"/>
+    <hyperlink ref="G68" r:id="rId134" display="http://www.hcltech.com/" xr:uid="{00000000-0004-0000-0200-000085000000}"/>
+    <hyperlink ref="F69" r:id="rId135" display="https://www.forbes.com/companies/fujitsu-america/?list=best-management-consulting-firms" xr:uid="{00000000-0004-0000-0200-000086000000}"/>
+    <hyperlink ref="G69" r:id="rId136" display="http://www.fujitsu.com/" xr:uid="{00000000-0004-0000-0200-000087000000}"/>
+    <hyperlink ref="F70" r:id="rId137" display="https://www.forbes.com/companies/bridge-solutions-group/?list=best-management-consulting-firms" xr:uid="{00000000-0004-0000-0200-000088000000}"/>
+    <hyperlink ref="G70" r:id="rId138" display="http://bridgesgi.com/" xr:uid="{00000000-0004-0000-0200-000089000000}"/>
+    <hyperlink ref="F71" r:id="rId139" display="https://www.forbes.com/companies/blue-horseshoe-solutions/?list=best-management-consulting-firms" xr:uid="{00000000-0004-0000-0200-00008A000000}"/>
+    <hyperlink ref="G71" r:id="rId140" display="http://www.bhsolutions.com/" xr:uid="{00000000-0004-0000-0200-00008B000000}"/>
+    <hyperlink ref="F72" r:id="rId141" display="https://www.forbes.com/companies/application-consulting-group/?list=best-management-consulting-firms" xr:uid="{00000000-0004-0000-0200-00008C000000}"/>
+    <hyperlink ref="G72" r:id="rId142" display="http://www.acgi.com/" xr:uid="{00000000-0004-0000-0200-00008D000000}"/>
+    <hyperlink ref="F73" r:id="rId143" display="https://www.forbes.com/companies/simon-kucher-partners/?list=best-management-consulting-firms" xr:uid="{00000000-0004-0000-0200-00008E000000}"/>
+    <hyperlink ref="G73" r:id="rId144" display="http://www.simon-kucher.com/" xr:uid="{00000000-0004-0000-0200-00008F000000}"/>
+    <hyperlink ref="F74" r:id="rId145" display="https://www.forbes.com/companies/navigant-consulting/?list=best-management-consulting-firms" xr:uid="{00000000-0004-0000-0200-000090000000}"/>
+    <hyperlink ref="G74" r:id="rId146" display="http://www.navigant.com/" xr:uid="{00000000-0004-0000-0200-000091000000}"/>
+    <hyperlink ref="F75" r:id="rId147" display="https://www.forbes.com/companies/keystone-strategy/?list=best-management-consulting-firms" xr:uid="{00000000-0004-0000-0200-000092000000}"/>
+    <hyperlink ref="G75" r:id="rId148" display="http://www.keystonestrategy.com/" xr:uid="{00000000-0004-0000-0200-000093000000}"/>
+    <hyperlink ref="F76" r:id="rId149" display="https://www.forbes.com/companies/kaiser-associates/?list=best-management-consulting-firms" xr:uid="{00000000-0004-0000-0200-000094000000}"/>
+    <hyperlink ref="G76" r:id="rId150" display="http://www.kaiserassociates.com/" xr:uid="{00000000-0004-0000-0200-000095000000}"/>
+    <hyperlink ref="F77" r:id="rId151" display="https://www.forbes.com/companies/insight-sourcing-group/?list=best-management-consulting-firms" xr:uid="{00000000-0004-0000-0200-000096000000}"/>
+    <hyperlink ref="G77" r:id="rId152" display="http://www.insightsourcing.com/" xr:uid="{00000000-0004-0000-0200-000097000000}"/>
+    <hyperlink ref="F78" r:id="rId153" display="https://www.forbes.com/companies/innosight/?list=best-management-consulting-firms" xr:uid="{00000000-0004-0000-0200-000098000000}"/>
+    <hyperlink ref="G78" r:id="rId154" display="http://www.innosight.com/" xr:uid="{00000000-0004-0000-0200-000099000000}"/>
+    <hyperlink ref="F79" r:id="rId155" display="https://www.forbes.com/companies/ibb-consulting-group/?list=best-management-consulting-firms" xr:uid="{00000000-0004-0000-0200-00009A000000}"/>
+    <hyperlink ref="G79" r:id="rId156" display="http://www.ibbconsulting.com/" xr:uid="{00000000-0004-0000-0200-00009B000000}"/>
+    <hyperlink ref="F80" r:id="rId157" display="https://www.forbes.com/companies/hay-group/?list=best-management-consulting-firms" xr:uid="{00000000-0004-0000-0200-00009C000000}"/>
+    <hyperlink ref="G80" r:id="rId158" display="http://www.haygroup.com/" xr:uid="{00000000-0004-0000-0200-00009D000000}"/>
+    <hyperlink ref="F81" r:id="rId159" display="https://www.forbes.com/companies/cornerstone-research/?list=best-management-consulting-firms" xr:uid="{00000000-0004-0000-0200-00009E000000}"/>
+    <hyperlink ref="G81" r:id="rId160" display="http://www.cornerstone.com/" xr:uid="{00000000-0004-0000-0200-00009F000000}"/>
+    <hyperlink ref="F82" r:id="rId161" display="https://www.forbes.com/companies/charles-river-associates/?list=best-management-consulting-firms" xr:uid="{00000000-0004-0000-0200-0000A0000000}"/>
+    <hyperlink ref="G82" r:id="rId162" display="http://www.crai.com/" xr:uid="{00000000-0004-0000-0200-0000A1000000}"/>
+    <hyperlink ref="F83" r:id="rId163" display="https://www.forbes.com/companies/centric-consulting/?list=best-management-consulting-firms" xr:uid="{00000000-0004-0000-0200-0000A2000000}"/>
+    <hyperlink ref="G83" r:id="rId164" display="http://www.centricconsulting.com/" xr:uid="{00000000-0004-0000-0200-0000A3000000}"/>
+    <hyperlink ref="F84" r:id="rId165" display="https://www.forbes.com/companies/bates-white/?list=best-management-consulting-firms" xr:uid="{00000000-0004-0000-0200-0000A4000000}"/>
+    <hyperlink ref="G84" r:id="rId166" display="http://www.bateswhite.com/" xr:uid="{00000000-0004-0000-0200-0000A5000000}"/>
+    <hyperlink ref="F85" r:id="rId167" display="https://www.forbes.com/companies/avanade/?list=best-management-consulting-firms" xr:uid="{00000000-0004-0000-0200-0000A6000000}"/>
+    <hyperlink ref="G85" r:id="rId168" display="http://www.avanade.com/" xr:uid="{00000000-0004-0000-0200-0000A7000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="D2:F52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="39.5703125" customWidth="1"/>
     <col min="6" max="6" width="55.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="4:6" ht="31.5">
+    <row r="2" spans="4:6" ht="34.5" x14ac:dyDescent="0.25">
       <c r="D2" s="12" t="s">
         <v>87</v>
       </c>
@@ -6636,7 +6647,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="4:6">
+    <row r="3" spans="4:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D3" s="13">
         <v>1</v>
       </c>
@@ -6647,7 +6658,7 @@
         <v>17310000000</v>
       </c>
     </row>
-    <row r="4" spans="4:6">
+    <row r="4" spans="4:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D4" s="13">
         <v>2</v>
       </c>
@@ -6658,7 +6669,7 @@
         <v>15460000000</v>
       </c>
     </row>
-    <row r="5" spans="4:6">
+    <row r="5" spans="4:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D5" s="13">
         <v>3</v>
       </c>
@@ -6669,7 +6680,7 @@
         <v>14930000000</v>
       </c>
     </row>
-    <row r="6" spans="4:6">
+    <row r="6" spans="4:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D6" s="13">
         <v>4</v>
       </c>
@@ -6680,7 +6691,7 @@
         <v>14810000000</v>
       </c>
     </row>
-    <row r="7" spans="4:6">
+    <row r="7" spans="4:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D7" s="13">
         <v>5</v>
       </c>
@@ -6691,7 +6702,7 @@
         <v>13350000000</v>
       </c>
     </row>
-    <row r="8" spans="4:6">
+    <row r="8" spans="4:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D8" s="13">
         <v>6</v>
       </c>
@@ -6702,7 +6713,7 @@
         <v>12253000000</v>
       </c>
     </row>
-    <row r="9" spans="4:6">
+    <row r="9" spans="4:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D9" s="13">
         <v>7</v>
       </c>
@@ -6713,7 +6724,7 @@
         <v>12000000000</v>
       </c>
     </row>
-    <row r="10" spans="4:6">
+    <row r="10" spans="4:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D10" s="13">
         <v>8</v>
       </c>
@@ -6724,7 +6735,7 @@
         <v>11600000000</v>
       </c>
     </row>
-    <row r="11" spans="4:6">
+    <row r="11" spans="4:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D11" s="13">
         <v>9</v>
       </c>
@@ -6735,7 +6746,7 @@
         <v>10210000000</v>
       </c>
     </row>
-    <row r="12" spans="4:6">
+    <row r="12" spans="4:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D12" s="13">
         <v>10</v>
       </c>
@@ -6746,7 +6757,7 @@
         <v>10180000000</v>
       </c>
     </row>
-    <row r="13" spans="4:6">
+    <row r="13" spans="4:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D13" s="13">
         <v>11</v>
       </c>
@@ -6757,7 +6768,7 @@
         <v>8800000000</v>
       </c>
     </row>
-    <row r="14" spans="4:6">
+    <row r="14" spans="4:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D14" s="13">
         <v>12</v>
       </c>
@@ -6768,7 +6779,7 @@
         <v>8500000000</v>
       </c>
     </row>
-    <row r="15" spans="4:6">
+    <row r="15" spans="4:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D15" s="13">
         <v>13</v>
       </c>
@@ -6779,7 +6790,7 @@
         <v>7882000000</v>
       </c>
     </row>
-    <row r="16" spans="4:6">
+    <row r="16" spans="4:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D16" s="13">
         <v>14</v>
       </c>
@@ -6790,7 +6801,7 @@
         <v>6300000000</v>
       </c>
     </row>
-    <row r="17" spans="4:6">
+    <row r="17" spans="4:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D17" s="13">
         <v>15</v>
       </c>
@@ -6801,7 +6812,7 @@
         <v>6100000000</v>
       </c>
     </row>
-    <row r="18" spans="4:6">
+    <row r="18" spans="4:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D18" s="13">
         <v>16</v>
       </c>
@@ -6812,7 +6823,7 @@
         <v>4300000000</v>
       </c>
     </row>
-    <row r="19" spans="4:6">
+    <row r="19" spans="4:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D19" s="13">
         <v>17</v>
       </c>
@@ -6823,7 +6834,7 @@
         <v>4200000000</v>
       </c>
     </row>
-    <row r="20" spans="4:6">
+    <row r="20" spans="4:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D20" s="13">
         <v>18</v>
       </c>
@@ -6834,7 +6845,7 @@
         <v>3870000000</v>
       </c>
     </row>
-    <row r="21" spans="4:6">
+    <row r="21" spans="4:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D21" s="13">
         <v>19</v>
       </c>
@@ -6845,7 +6856,7 @@
         <v>3566000000</v>
       </c>
     </row>
-    <row r="22" spans="4:6">
+    <row r="22" spans="4:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D22" s="13">
         <v>20</v>
       </c>
@@ -6856,7 +6867,7 @@
         <v>3358000000</v>
       </c>
     </row>
-    <row r="23" spans="4:6">
+    <row r="23" spans="4:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D23" s="13">
         <v>21</v>
       </c>
@@ -6867,7 +6878,7 @@
         <v>3300000000</v>
       </c>
     </row>
-    <row r="24" spans="4:6">
+    <row r="24" spans="4:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D24" s="13">
         <v>22</v>
       </c>
@@ -6878,7 +6889,7 @@
         <v>2813000000</v>
       </c>
     </row>
-    <row r="25" spans="4:6">
+    <row r="25" spans="4:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D25" s="13">
         <v>23</v>
       </c>
@@ -6889,7 +6900,7 @@
         <v>2000000000</v>
       </c>
     </row>
-    <row r="26" spans="4:6">
+    <row r="26" spans="4:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D26" s="13">
         <v>24</v>
       </c>
@@ -6900,7 +6911,7 @@
         <v>1800000000</v>
       </c>
     </row>
-    <row r="27" spans="4:6">
+    <row r="27" spans="4:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D27" s="13">
         <v>25</v>
       </c>
@@ -6911,7 +6922,7 @@
         <v>1800000000</v>
       </c>
     </row>
-    <row r="28" spans="4:6">
+    <row r="28" spans="4:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D28" s="13">
         <v>26</v>
       </c>
@@ -6922,7 +6933,7 @@
         <v>1700000000</v>
       </c>
     </row>
-    <row r="29" spans="4:6">
+    <row r="29" spans="4:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D29" s="13">
         <v>27</v>
       </c>
@@ -6933,7 +6944,7 @@
         <v>1410000000</v>
       </c>
     </row>
-    <row r="30" spans="4:6">
+    <row r="30" spans="4:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D30" s="13">
         <v>28</v>
       </c>
@@ -6944,7 +6955,7 @@
         <v>1400000000</v>
       </c>
     </row>
-    <row r="31" spans="4:6">
+    <row r="31" spans="4:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D31" s="13">
         <v>29</v>
       </c>
@@ -6955,7 +6966,7 @@
         <v>1305000000</v>
       </c>
     </row>
-    <row r="32" spans="4:6">
+    <row r="32" spans="4:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D32" s="13">
         <v>30</v>
       </c>
@@ -6966,7 +6977,7 @@
         <v>1300000000</v>
       </c>
     </row>
-    <row r="33" spans="4:6">
+    <row r="33" spans="4:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D33" s="13">
         <v>31</v>
       </c>
@@ -6977,7 +6988,7 @@
         <v>1300000000</v>
       </c>
     </row>
-    <row r="34" spans="4:6">
+    <row r="34" spans="4:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D34" s="13">
         <v>32</v>
       </c>
@@ -6988,7 +6999,7 @@
         <v>1190000000</v>
       </c>
     </row>
-    <row r="35" spans="4:6">
+    <row r="35" spans="4:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D35" s="13">
         <v>33</v>
       </c>
@@ -6999,7 +7010,7 @@
         <v>1000000000</v>
       </c>
     </row>
-    <row r="36" spans="4:6">
+    <row r="36" spans="4:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D36" s="13">
         <v>34</v>
       </c>
@@ -7010,7 +7021,7 @@
         <v>1000000000</v>
       </c>
     </row>
-    <row r="37" spans="4:6">
+    <row r="37" spans="4:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D37" s="13">
         <v>35</v>
       </c>
@@ -7021,7 +7032,7 @@
         <v>1000000000</v>
       </c>
     </row>
-    <row r="38" spans="4:6">
+    <row r="38" spans="4:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D38" s="13">
         <v>36</v>
       </c>
@@ -7032,7 +7043,7 @@
         <v>816000000</v>
       </c>
     </row>
-    <row r="39" spans="4:6">
+    <row r="39" spans="4:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D39" s="13">
         <v>37</v>
       </c>
@@ -7043,7 +7054,7 @@
         <v>797700000</v>
       </c>
     </row>
-    <row r="40" spans="4:6">
+    <row r="40" spans="4:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D40" s="13">
         <v>38</v>
       </c>
@@ -7054,7 +7065,7 @@
         <v>781800000</v>
       </c>
     </row>
-    <row r="41" spans="4:6">
+    <row r="41" spans="4:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D41" s="13">
         <v>39</v>
       </c>
@@ -7065,7 +7076,7 @@
         <v>767000000</v>
       </c>
     </row>
-    <row r="42" spans="4:6">
+    <row r="42" spans="4:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D42" s="13">
         <v>40</v>
       </c>
@@ -7076,7 +7087,7 @@
         <v>600000000</v>
       </c>
     </row>
-    <row r="43" spans="4:6">
+    <row r="43" spans="4:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D43" s="13">
         <v>41</v>
       </c>
@@ -7087,7 +7098,7 @@
         <v>600000000</v>
       </c>
     </row>
-    <row r="44" spans="4:6">
+    <row r="44" spans="4:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D44" s="13">
         <v>42</v>
       </c>
@@ -7098,7 +7109,7 @@
         <v>556000000</v>
       </c>
     </row>
-    <row r="45" spans="4:6">
+    <row r="45" spans="4:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D45" s="13">
         <v>43</v>
       </c>
@@ -7109,7 +7120,7 @@
         <v>525000000</v>
       </c>
     </row>
-    <row r="46" spans="4:6">
+    <row r="46" spans="4:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D46" s="13">
         <v>44</v>
       </c>
@@ -7120,7 +7131,7 @@
         <v>500000000</v>
       </c>
     </row>
-    <row r="47" spans="4:6">
+    <row r="47" spans="4:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D47" s="13">
         <v>45</v>
       </c>
@@ -7131,7 +7142,7 @@
         <v>487000000</v>
       </c>
     </row>
-    <row r="48" spans="4:6">
+    <row r="48" spans="4:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D48" s="13">
         <v>46</v>
       </c>
@@ -7142,7 +7153,7 @@
         <v>311000000</v>
       </c>
     </row>
-    <row r="49" spans="4:6">
+    <row r="49" spans="4:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D49" s="13">
         <v>47</v>
       </c>
@@ -7153,7 +7164,7 @@
         <v>239200000</v>
       </c>
     </row>
-    <row r="50" spans="4:6">
+    <row r="50" spans="4:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D50" s="13">
         <v>48</v>
       </c>
@@ -7164,7 +7175,7 @@
         <v>200000000</v>
       </c>
     </row>
-    <row r="51" spans="4:6">
+    <row r="51" spans="4:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D51" s="13">
         <v>49</v>
       </c>
@@ -7175,7 +7186,7 @@
         <v>162000000</v>
       </c>
     </row>
-    <row r="52" spans="4:6">
+    <row r="52" spans="4:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D52" s="15">
         <v>50</v>
       </c>
@@ -7192,16 +7203,16 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="7" spans="7:7">
+    <row r="7" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G7" t="s">
         <v>86</v>
       </c>

</xml_diff>